<commit_message>
Nondescript commit message done purposefully for frustration
</commit_message>
<xml_diff>
--- a/RESOURCES/Project Backlog .xlsx
+++ b/RESOURCES/Project Backlog .xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>Stock Viewer Backlog</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Valerian Salh</t>
   </si>
 </sst>
 </file>
@@ -548,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -575,12 +578,12 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="12.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -589,7 +592,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="12.75">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -615,7 +618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="12.75">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -639,7 +642,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="12.75">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -663,7 +666,7 @@
       </c>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="12.75">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
@@ -687,7 +690,7 @@
       </c>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="12.75">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -711,7 +714,7 @@
       </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="12.75">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -735,7 +738,7 @@
       </c>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="12.75">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -759,7 +762,7 @@
       </c>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="12.75">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -783,7 +786,7 @@
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="12.75">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -807,7 +810,7 @@
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="12.75">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -831,7 +834,7 @@
       </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="12.75">
       <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
@@ -855,7 +858,7 @@
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="12.75">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -879,7 +882,7 @@
       </c>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="12.75">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
@@ -903,7 +906,7 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="12.75">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -927,7 +930,7 @@
       </c>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="12.75">
       <c r="A17" s="11"/>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
@@ -937,7 +940,7 @@
       <c r="G17" s="12"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="12.75">
       <c r="A18" s="11"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
@@ -947,7 +950,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="12.75">
       <c r="A19" s="11"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
@@ -957,7 +960,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="12.75">
       <c r="A20" s="11"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
@@ -967,7 +970,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="12.75">
       <c r="A21" s="11"/>
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
@@ -977,7 +980,7 @@
       <c r="G21" s="12"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="12.75">
       <c r="A22" s="11"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
@@ -987,7 +990,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="12.75">
       <c r="A23" s="11"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -997,7 +1000,7 @@
       <c r="G23" s="12"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="12.75">
       <c r="A24" s="11"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
@@ -1007,7 +1010,7 @@
       <c r="G24" s="12"/>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="12.75">
       <c r="A25" s="11"/>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
@@ -1017,7 +1020,7 @@
       <c r="G25" s="12"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="12.75">
       <c r="A26" s="11"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
@@ -1027,7 +1030,7 @@
       <c r="G26" s="12"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="12.75">
       <c r="A27" s="11"/>
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
@@ -1037,7 +1040,7 @@
       <c r="G27" s="12"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="12.75">
       <c r="A28" s="11"/>
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
@@ -1047,7 +1050,7 @@
       <c r="G28" s="12"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="12.75">
       <c r="A29" s="11"/>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
@@ -1057,7 +1060,7 @@
       <c r="G29" s="12"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="12.75">
       <c r="A30" s="11"/>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
@@ -1067,7 +1070,7 @@
       <c r="G30" s="12"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" ht="12.75">
       <c r="A31" s="11"/>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
@@ -1077,7 +1080,7 @@
       <c r="G31" s="12"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" ht="12.75">
       <c r="A32" s="11"/>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
@@ -1087,7 +1090,7 @@
       <c r="G32" s="12"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="12.75">
       <c r="A33" s="11"/>
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
@@ -1097,7 +1100,7 @@
       <c r="G33" s="12"/>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="12.75">
       <c r="A34" s="11"/>
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
@@ -1107,7 +1110,7 @@
       <c r="G34" s="12"/>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="12.75">
       <c r="A35" s="11"/>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
@@ -1117,7 +1120,7 @@
       <c r="G35" s="12"/>
       <c r="H35" s="10"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" ht="12.75">
       <c r="A36" s="11"/>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
@@ -1127,7 +1130,7 @@
       <c r="G36" s="12"/>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" ht="12.75">
       <c r="A37" s="11"/>
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
@@ -1137,7 +1140,7 @@
       <c r="G37" s="12"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" ht="12.75">
       <c r="A38" s="11"/>
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
@@ -1147,7 +1150,7 @@
       <c r="G38" s="12"/>
       <c r="H38" s="10"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="12.75">
       <c r="A39" s="11"/>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
@@ -1157,7 +1160,7 @@
       <c r="G39" s="12"/>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" ht="12.75">
       <c r="A40" s="11"/>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
@@ -1167,7 +1170,7 @@
       <c r="G40" s="12"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" ht="12.75">
       <c r="A41" s="11"/>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
@@ -1177,7 +1180,7 @@
       <c r="G41" s="12"/>
       <c r="H41" s="10"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" ht="12.75">
       <c r="A42" s="11"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
@@ -1187,7 +1190,7 @@
       <c r="G42" s="12"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" ht="12.75">
       <c r="A43" s="11"/>
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
@@ -1197,7 +1200,7 @@
       <c r="G43" s="12"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" ht="12.75">
       <c r="A44" s="11"/>
       <c r="B44" s="10"/>
       <c r="C44" s="11"/>
@@ -1207,7 +1210,7 @@
       <c r="G44" s="12"/>
       <c r="H44" s="10"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" ht="12.75">
       <c r="A45" s="11"/>
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
@@ -1217,7 +1220,7 @@
       <c r="G45" s="12"/>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" ht="12.75">
       <c r="A46" s="11"/>
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
@@ -1227,7 +1230,7 @@
       <c r="G46" s="12"/>
       <c r="H46" s="10"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" ht="12.75">
       <c r="A47" s="11"/>
       <c r="B47" s="10"/>
       <c r="C47" s="11"/>
@@ -1237,7 +1240,7 @@
       <c r="G47" s="12"/>
       <c r="H47" s="10"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" ht="12.75">
       <c r="A48" s="11"/>
       <c r="B48" s="10"/>
       <c r="C48" s="11"/>
@@ -1247,7 +1250,7 @@
       <c r="G48" s="12"/>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" ht="12.75">
       <c r="A49" s="11"/>
       <c r="B49" s="10"/>
       <c r="C49" s="11"/>
@@ -1257,7 +1260,7 @@
       <c r="G49" s="12"/>
       <c r="H49" s="10"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" ht="12.75">
       <c r="A50" s="11"/>
       <c r="B50" s="10"/>
       <c r="C50" s="11"/>
@@ -1267,7 +1270,7 @@
       <c r="G50" s="12"/>
       <c r="H50" s="10"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" ht="12.75">
       <c r="A51" s="11"/>
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
@@ -1277,7 +1280,7 @@
       <c r="G51" s="12"/>
       <c r="H51" s="10"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" ht="12.75">
       <c r="A52" s="11"/>
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
@@ -1287,7 +1290,7 @@
       <c r="G52" s="12"/>
       <c r="H52" s="10"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" ht="12.75">
       <c r="A53" s="11"/>
       <c r="B53" s="10"/>
       <c r="C53" s="11"/>
@@ -1297,7 +1300,7 @@
       <c r="G53" s="12"/>
       <c r="H53" s="10"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" ht="12.75">
       <c r="A54" s="11"/>
       <c r="B54" s="10"/>
       <c r="C54" s="11"/>
@@ -1307,7 +1310,7 @@
       <c r="G54" s="12"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" ht="12.75">
       <c r="A55" s="11"/>
       <c r="B55" s="10"/>
       <c r="C55" s="11"/>
@@ -1317,7 +1320,7 @@
       <c r="G55" s="12"/>
       <c r="H55" s="10"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" ht="12.75">
       <c r="A56" s="11"/>
       <c r="B56" s="10"/>
       <c r="C56" s="11"/>
@@ -1327,7 +1330,7 @@
       <c r="G56" s="12"/>
       <c r="H56" s="10"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" ht="12.75">
       <c r="A57" s="11"/>
       <c r="B57" s="10"/>
       <c r="C57" s="11"/>
@@ -1337,7 +1340,7 @@
       <c r="G57" s="12"/>
       <c r="H57" s="10"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" ht="12.75">
       <c r="A58" s="11"/>
       <c r="B58" s="10"/>
       <c r="C58" s="11"/>
@@ -1347,7 +1350,7 @@
       <c r="G58" s="12"/>
       <c r="H58" s="10"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" ht="12.75">
       <c r="A59" s="11"/>
       <c r="B59" s="10"/>
       <c r="C59" s="11"/>
@@ -1357,7 +1360,7 @@
       <c r="G59" s="12"/>
       <c r="H59" s="10"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" ht="12.75">
       <c r="A60" s="11"/>
       <c r="B60" s="10"/>
       <c r="C60" s="11"/>
@@ -1367,7 +1370,7 @@
       <c r="G60" s="12"/>
       <c r="H60" s="10"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" ht="12.75">
       <c r="A61" s="11"/>
       <c r="B61" s="10"/>
       <c r="C61" s="11"/>
@@ -1377,7 +1380,7 @@
       <c r="G61" s="12"/>
       <c r="H61" s="10"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" ht="12.75">
       <c r="A62" s="11"/>
       <c r="B62" s="10"/>
       <c r="C62" s="11"/>
@@ -1387,7 +1390,7 @@
       <c r="G62" s="12"/>
       <c r="H62" s="10"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" ht="12.75">
       <c r="A63" s="11"/>
       <c r="B63" s="10"/>
       <c r="C63" s="11"/>
@@ -1397,7 +1400,7 @@
       <c r="G63" s="12"/>
       <c r="H63" s="10"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" ht="12.75">
       <c r="A64" s="11"/>
       <c r="B64" s="10"/>
       <c r="C64" s="11"/>
@@ -1407,7 +1410,7 @@
       <c r="G64" s="12"/>
       <c r="H64" s="10"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" ht="12.75">
       <c r="A65" s="11"/>
       <c r="B65" s="10"/>
       <c r="C65" s="11"/>
@@ -1417,7 +1420,7 @@
       <c r="G65" s="12"/>
       <c r="H65" s="10"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" ht="12.75">
       <c r="A66" s="11"/>
       <c r="B66" s="10"/>
       <c r="C66" s="11"/>
@@ -1427,7 +1430,7 @@
       <c r="G66" s="12"/>
       <c r="H66" s="10"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" ht="12.75">
       <c r="A67" s="11"/>
       <c r="B67" s="10"/>
       <c r="C67" s="11"/>
@@ -1437,7 +1440,7 @@
       <c r="G67" s="12"/>
       <c r="H67" s="10"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" ht="12.75">
       <c r="A68" s="11"/>
       <c r="B68" s="10"/>
       <c r="C68" s="11"/>
@@ -1447,7 +1450,7 @@
       <c r="G68" s="12"/>
       <c r="H68" s="10"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" ht="12.75">
       <c r="A69" s="11"/>
       <c r="B69" s="10"/>
       <c r="C69" s="11"/>
@@ -1457,7 +1460,7 @@
       <c r="G69" s="12"/>
       <c r="H69" s="10"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" ht="12.75">
       <c r="A70" s="11"/>
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
@@ -1467,7 +1470,7 @@
       <c r="G70" s="12"/>
       <c r="H70" s="10"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" ht="12.75">
       <c r="A71" s="11"/>
       <c r="B71" s="10"/>
       <c r="C71" s="11"/>
@@ -1477,7 +1480,7 @@
       <c r="G71" s="12"/>
       <c r="H71" s="10"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" ht="12.75">
       <c r="A72" s="11"/>
       <c r="B72" s="10"/>
       <c r="C72" s="11"/>
@@ -1487,7 +1490,7 @@
       <c r="G72" s="12"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" ht="12.75">
       <c r="A73" s="11"/>
       <c r="B73" s="10"/>
       <c r="C73" s="11"/>
@@ -1497,7 +1500,7 @@
       <c r="G73" s="12"/>
       <c r="H73" s="10"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" ht="12.75">
       <c r="A74" s="11"/>
       <c r="B74" s="10"/>
       <c r="C74" s="11"/>
@@ -1507,7 +1510,7 @@
       <c r="G74" s="12"/>
       <c r="H74" s="10"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" ht="12.75">
       <c r="A75" s="11"/>
       <c r="B75" s="10"/>
       <c r="C75" s="11"/>
@@ -1517,7 +1520,7 @@
       <c r="G75" s="12"/>
       <c r="H75" s="10"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" ht="12.75">
       <c r="A76" s="11"/>
       <c r="B76" s="10"/>
       <c r="C76" s="11"/>
@@ -1527,7 +1530,7 @@
       <c r="G76" s="12"/>
       <c r="H76" s="10"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" ht="12.75">
       <c r="A77" s="11"/>
       <c r="B77" s="10"/>
       <c r="C77" s="11"/>
@@ -1537,7 +1540,7 @@
       <c r="G77" s="12"/>
       <c r="H77" s="10"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" ht="12.75">
       <c r="A78" s="11"/>
       <c r="B78" s="10"/>
       <c r="C78" s="11"/>
@@ -1547,7 +1550,7 @@
       <c r="G78" s="12"/>
       <c r="H78" s="10"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" ht="12.75">
       <c r="A79" s="11"/>
       <c r="B79" s="10"/>
       <c r="C79" s="11"/>
@@ -1557,7 +1560,7 @@
       <c r="G79" s="12"/>
       <c r="H79" s="10"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" ht="12.75">
       <c r="A80" s="11"/>
       <c r="B80" s="10"/>
       <c r="C80" s="11"/>
@@ -1567,7 +1570,7 @@
       <c r="G80" s="12"/>
       <c r="H80" s="10"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" ht="12.75">
       <c r="A81" s="11"/>
       <c r="B81" s="10"/>
       <c r="C81" s="11"/>
@@ -1577,7 +1580,7 @@
       <c r="G81" s="12"/>
       <c r="H81" s="10"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" ht="12.75">
       <c r="A82" s="11"/>
       <c r="B82" s="10"/>
       <c r="C82" s="11"/>
@@ -1587,7 +1590,7 @@
       <c r="G82" s="12"/>
       <c r="H82" s="10"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" ht="12.75">
       <c r="A83" s="11"/>
       <c r="B83" s="10"/>
       <c r="C83" s="11"/>
@@ -1597,7 +1600,7 @@
       <c r="G83" s="12"/>
       <c r="H83" s="10"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" ht="12.75">
       <c r="A84" s="11"/>
       <c r="B84" s="10"/>
       <c r="C84" s="11"/>
@@ -1607,7 +1610,7 @@
       <c r="G84" s="12"/>
       <c r="H84" s="10"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" ht="12.75">
       <c r="A85" s="11"/>
       <c r="B85" s="10"/>
       <c r="C85" s="11"/>
@@ -1617,7 +1620,7 @@
       <c r="G85" s="12"/>
       <c r="H85" s="10"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" ht="12.75">
       <c r="A86" s="11"/>
       <c r="B86" s="10"/>
       <c r="C86" s="11"/>
@@ -1627,7 +1630,7 @@
       <c r="G86" s="12"/>
       <c r="H86" s="10"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" ht="12.75">
       <c r="A87" s="11"/>
       <c r="B87" s="10"/>
       <c r="C87" s="11"/>
@@ -1637,7 +1640,7 @@
       <c r="G87" s="12"/>
       <c r="H87" s="10"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" ht="12.75">
       <c r="A88" s="11"/>
       <c r="B88" s="10"/>
       <c r="C88" s="11"/>
@@ -1647,7 +1650,7 @@
       <c r="G88" s="12"/>
       <c r="H88" s="10"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" ht="12.75">
       <c r="A89" s="11"/>
       <c r="B89" s="10"/>
       <c r="C89" s="11"/>
@@ -1657,7 +1660,7 @@
       <c r="G89" s="12"/>
       <c r="H89" s="10"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" ht="12.75">
       <c r="A90" s="11"/>
       <c r="B90" s="10"/>
       <c r="C90" s="11"/>
@@ -1667,7 +1670,7 @@
       <c r="G90" s="12"/>
       <c r="H90" s="10"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" ht="12.75">
       <c r="A91" s="11"/>
       <c r="B91" s="10"/>
       <c r="C91" s="11"/>
@@ -1677,7 +1680,7 @@
       <c r="G91" s="12"/>
       <c r="H91" s="10"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" ht="12.75">
       <c r="A92" s="11"/>
       <c r="B92" s="10"/>
       <c r="C92" s="11"/>
@@ -1687,7 +1690,7 @@
       <c r="G92" s="12"/>
       <c r="H92" s="10"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" ht="12.75">
       <c r="A93" s="11"/>
       <c r="B93" s="10"/>
       <c r="C93" s="11"/>
@@ -1697,7 +1700,7 @@
       <c r="G93" s="12"/>
       <c r="H93" s="10"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" ht="12.75">
       <c r="A94" s="11"/>
       <c r="B94" s="10"/>
       <c r="C94" s="11"/>
@@ -1707,7 +1710,7 @@
       <c r="G94" s="12"/>
       <c r="H94" s="10"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" ht="12.75">
       <c r="A95" s="11"/>
       <c r="B95" s="10"/>
       <c r="C95" s="11"/>
@@ -1717,7 +1720,7 @@
       <c r="G95" s="12"/>
       <c r="H95" s="10"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" ht="12.75">
       <c r="A96" s="11"/>
       <c r="B96" s="10"/>
       <c r="C96" s="11"/>
@@ -1727,7 +1730,7 @@
       <c r="G96" s="12"/>
       <c r="H96" s="10"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" ht="12.75">
       <c r="A97" s="11"/>
       <c r="B97" s="10"/>
       <c r="C97" s="11"/>
@@ -1737,7 +1740,7 @@
       <c r="G97" s="12"/>
       <c r="H97" s="10"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" ht="12.75">
       <c r="A98" s="11"/>
       <c r="B98" s="10"/>
       <c r="C98" s="11"/>
@@ -1747,7 +1750,7 @@
       <c r="G98" s="12"/>
       <c r="H98" s="10"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" ht="12.75">
       <c r="A99" s="11"/>
       <c r="B99" s="10"/>
       <c r="C99" s="11"/>
@@ -1757,7 +1760,7 @@
       <c r="G99" s="12"/>
       <c r="H99" s="10"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" ht="12.75">
       <c r="A100" s="11"/>
       <c r="B100" s="10"/>
       <c r="C100" s="11"/>
@@ -1767,7 +1770,7 @@
       <c r="G100" s="12"/>
       <c r="H100" s="10"/>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" ht="12.75">
       <c r="A101" s="11"/>
       <c r="B101" s="10"/>
       <c r="C101" s="11"/>
@@ -1777,7 +1780,7 @@
       <c r="G101" s="12"/>
       <c r="H101" s="10"/>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" ht="12.75">
       <c r="A102" s="11"/>
       <c r="B102" s="10"/>
       <c r="C102" s="11"/>
@@ -1787,7 +1790,7 @@
       <c r="G102" s="12"/>
       <c r="H102" s="10"/>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" ht="12.75">
       <c r="A103" s="11"/>
       <c r="B103" s="10"/>
       <c r="C103" s="11"/>
@@ -1797,7 +1800,7 @@
       <c r="G103" s="12"/>
       <c r="H103" s="10"/>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" ht="12.75">
       <c r="A104" s="11"/>
       <c r="B104" s="10"/>
       <c r="C104" s="11"/>
@@ -1807,7 +1810,7 @@
       <c r="G104" s="12"/>
       <c r="H104" s="10"/>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" ht="12.75">
       <c r="A105" s="11"/>
       <c r="B105" s="10"/>
       <c r="C105" s="11"/>
@@ -1817,7 +1820,7 @@
       <c r="G105" s="12"/>
       <c r="H105" s="10"/>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" ht="12.75">
       <c r="A106" s="11"/>
       <c r="B106" s="10"/>
       <c r="C106" s="11"/>
@@ -1827,7 +1830,7 @@
       <c r="G106" s="12"/>
       <c r="H106" s="10"/>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" ht="12.75">
       <c r="A107" s="11"/>
       <c r="B107" s="10"/>
       <c r="C107" s="11"/>
@@ -1837,7 +1840,7 @@
       <c r="G107" s="12"/>
       <c r="H107" s="10"/>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" ht="12.75">
       <c r="A108" s="11"/>
       <c r="B108" s="10"/>
       <c r="C108" s="11"/>
@@ -1847,7 +1850,7 @@
       <c r="G108" s="12"/>
       <c r="H108" s="10"/>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" ht="12.75">
       <c r="A109" s="11"/>
       <c r="B109" s="10"/>
       <c r="C109" s="11"/>
@@ -1857,7 +1860,7 @@
       <c r="G109" s="12"/>
       <c r="H109" s="10"/>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" ht="12.75">
       <c r="A110" s="11"/>
       <c r="B110" s="10"/>
       <c r="C110" s="11"/>
@@ -1867,7 +1870,7 @@
       <c r="G110" s="12"/>
       <c r="H110" s="10"/>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" ht="12.75">
       <c r="A111" s="11"/>
       <c r="B111" s="10"/>
       <c r="C111" s="11"/>
@@ -1877,7 +1880,7 @@
       <c r="G111" s="12"/>
       <c r="H111" s="10"/>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" ht="12.75">
       <c r="A112" s="11"/>
       <c r="B112" s="10"/>
       <c r="C112" s="11"/>
@@ -1887,7 +1890,7 @@
       <c r="G112" s="12"/>
       <c r="H112" s="10"/>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" ht="12.75">
       <c r="A113" s="11"/>
       <c r="B113" s="10"/>
       <c r="C113" s="11"/>
@@ -1897,7 +1900,7 @@
       <c r="G113" s="12"/>
       <c r="H113" s="10"/>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" ht="12.75">
       <c r="A114" s="11"/>
       <c r="B114" s="10"/>
       <c r="C114" s="11"/>
@@ -1907,7 +1910,7 @@
       <c r="G114" s="12"/>
       <c r="H114" s="10"/>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" ht="12.75">
       <c r="A115" s="11"/>
       <c r="B115" s="10"/>
       <c r="C115" s="11"/>
@@ -1917,7 +1920,7 @@
       <c r="G115" s="12"/>
       <c r="H115" s="10"/>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" ht="12.75">
       <c r="A116" s="11"/>
       <c r="B116" s="10"/>
       <c r="C116" s="11"/>
@@ -1927,7 +1930,7 @@
       <c r="G116" s="12"/>
       <c r="H116" s="10"/>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" ht="12.75">
       <c r="A117" s="11"/>
       <c r="B117" s="10"/>
       <c r="C117" s="11"/>
@@ -1937,7 +1940,7 @@
       <c r="G117" s="12"/>
       <c r="H117" s="10"/>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" ht="12.75">
       <c r="A118" s="11"/>
       <c r="B118" s="10"/>
       <c r="C118" s="11"/>
@@ -1947,7 +1950,7 @@
       <c r="G118" s="12"/>
       <c r="H118" s="10"/>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" ht="12.75">
       <c r="A119" s="11"/>
       <c r="B119" s="10"/>
       <c r="C119" s="11"/>
@@ -1957,7 +1960,7 @@
       <c r="G119" s="12"/>
       <c r="H119" s="10"/>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" ht="12.75">
       <c r="A120" s="11"/>
       <c r="B120" s="10"/>
       <c r="C120" s="11"/>
@@ -1967,7 +1970,7 @@
       <c r="G120" s="12"/>
       <c r="H120" s="10"/>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" ht="12.75">
       <c r="A121" s="11"/>
       <c r="B121" s="10"/>
       <c r="C121" s="11"/>
@@ -1977,7 +1980,7 @@
       <c r="G121" s="12"/>
       <c r="H121" s="10"/>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" ht="12.75">
       <c r="A122" s="11"/>
       <c r="B122" s="10"/>
       <c r="C122" s="11"/>
@@ -1987,7 +1990,7 @@
       <c r="G122" s="12"/>
       <c r="H122" s="10"/>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" ht="12.75">
       <c r="A123" s="11"/>
       <c r="B123" s="10"/>
       <c r="C123" s="11"/>
@@ -1997,7 +2000,7 @@
       <c r="G123" s="12"/>
       <c r="H123" s="10"/>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" ht="12.75">
       <c r="A124" s="11"/>
       <c r="B124" s="10"/>
       <c r="C124" s="11"/>
@@ -2007,7 +2010,7 @@
       <c r="G124" s="12"/>
       <c r="H124" s="10"/>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" ht="12.75">
       <c r="A125" s="11"/>
       <c r="B125" s="10"/>
       <c r="C125" s="11"/>
@@ -2017,7 +2020,7 @@
       <c r="G125" s="12"/>
       <c r="H125" s="10"/>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" ht="12.75">
       <c r="A126" s="11"/>
       <c r="B126" s="10"/>
       <c r="C126" s="11"/>
@@ -2027,7 +2030,7 @@
       <c r="G126" s="12"/>
       <c r="H126" s="10"/>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" ht="12.75">
       <c r="A127" s="11"/>
       <c r="B127" s="10"/>
       <c r="C127" s="11"/>
@@ -2037,7 +2040,7 @@
       <c r="G127" s="12"/>
       <c r="H127" s="10"/>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" ht="12.75">
       <c r="A128" s="11"/>
       <c r="B128" s="10"/>
       <c r="C128" s="11"/>
@@ -2047,7 +2050,7 @@
       <c r="G128" s="12"/>
       <c r="H128" s="10"/>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" ht="12.75">
       <c r="A129" s="11"/>
       <c r="B129" s="10"/>
       <c r="C129" s="11"/>
@@ -2057,7 +2060,7 @@
       <c r="G129" s="12"/>
       <c r="H129" s="10"/>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" ht="12.75">
       <c r="A130" s="11"/>
       <c r="B130" s="10"/>
       <c r="C130" s="11"/>
@@ -2067,7 +2070,7 @@
       <c r="G130" s="12"/>
       <c r="H130" s="10"/>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" ht="12.75">
       <c r="A131" s="11"/>
       <c r="B131" s="10"/>
       <c r="C131" s="11"/>
@@ -2077,7 +2080,7 @@
       <c r="G131" s="12"/>
       <c r="H131" s="10"/>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" ht="12.75">
       <c r="A132" s="11"/>
       <c r="B132" s="10"/>
       <c r="C132" s="11"/>
@@ -2087,7 +2090,7 @@
       <c r="G132" s="12"/>
       <c r="H132" s="10"/>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" ht="12.75">
       <c r="A133" s="11"/>
       <c r="B133" s="10"/>
       <c r="C133" s="11"/>
@@ -2097,7 +2100,7 @@
       <c r="G133" s="12"/>
       <c r="H133" s="10"/>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" ht="12.75">
       <c r="A134" s="11"/>
       <c r="B134" s="10"/>
       <c r="C134" s="11"/>
@@ -2107,7 +2110,7 @@
       <c r="G134" s="12"/>
       <c r="H134" s="10"/>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" ht="12.75">
       <c r="A135" s="11"/>
       <c r="B135" s="10"/>
       <c r="C135" s="11"/>
@@ -2117,7 +2120,7 @@
       <c r="G135" s="12"/>
       <c r="H135" s="10"/>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" ht="12.75">
       <c r="A136" s="11"/>
       <c r="B136" s="10"/>
       <c r="C136" s="11"/>
@@ -2127,7 +2130,7 @@
       <c r="G136" s="12"/>
       <c r="H136" s="10"/>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" ht="12.75">
       <c r="A137" s="11"/>
       <c r="B137" s="10"/>
       <c r="C137" s="11"/>
@@ -2137,7 +2140,7 @@
       <c r="G137" s="12"/>
       <c r="H137" s="10"/>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" ht="12.75">
       <c r="A138" s="11"/>
       <c r="B138" s="10"/>
       <c r="C138" s="11"/>
@@ -2147,7 +2150,7 @@
       <c r="G138" s="12"/>
       <c r="H138" s="10"/>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" ht="12.75">
       <c r="A139" s="11"/>
       <c r="B139" s="10"/>
       <c r="C139" s="11"/>
@@ -2157,7 +2160,7 @@
       <c r="G139" s="12"/>
       <c r="H139" s="10"/>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" ht="12.75">
       <c r="A140" s="11"/>
       <c r="B140" s="10"/>
       <c r="C140" s="11"/>
@@ -2167,7 +2170,7 @@
       <c r="G140" s="12"/>
       <c r="H140" s="10"/>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" ht="12.75">
       <c r="A141" s="11"/>
       <c r="B141" s="10"/>
       <c r="C141" s="11"/>
@@ -2177,7 +2180,7 @@
       <c r="G141" s="12"/>
       <c r="H141" s="10"/>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" ht="12.75">
       <c r="A142" s="11"/>
       <c r="B142" s="10"/>
       <c r="C142" s="11"/>
@@ -2187,7 +2190,7 @@
       <c r="G142" s="12"/>
       <c r="H142" s="10"/>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" ht="12.75">
       <c r="A143" s="11"/>
       <c r="B143" s="10"/>
       <c r="C143" s="11"/>
@@ -2197,7 +2200,7 @@
       <c r="G143" s="12"/>
       <c r="H143" s="10"/>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" ht="12.75">
       <c r="A144" s="11"/>
       <c r="B144" s="10"/>
       <c r="C144" s="11"/>
@@ -2207,7 +2210,7 @@
       <c r="G144" s="12"/>
       <c r="H144" s="10"/>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" ht="12.75">
       <c r="A145" s="11"/>
       <c r="B145" s="10"/>
       <c r="C145" s="11"/>
@@ -2217,7 +2220,7 @@
       <c r="G145" s="12"/>
       <c r="H145" s="10"/>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" ht="12.75">
       <c r="A146" s="11"/>
       <c r="B146" s="10"/>
       <c r="C146" s="11"/>
@@ -2227,7 +2230,7 @@
       <c r="G146" s="12"/>
       <c r="H146" s="10"/>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" ht="12.75">
       <c r="A147" s="11"/>
       <c r="B147" s="10"/>
       <c r="C147" s="11"/>
@@ -2237,7 +2240,7 @@
       <c r="G147" s="12"/>
       <c r="H147" s="10"/>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" ht="12.75">
       <c r="A148" s="11"/>
       <c r="B148" s="10"/>
       <c r="C148" s="11"/>
@@ -2247,7 +2250,7 @@
       <c r="G148" s="12"/>
       <c r="H148" s="10"/>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" ht="12.75">
       <c r="A149" s="11"/>
       <c r="B149" s="10"/>
       <c r="C149" s="11"/>
@@ -2257,7 +2260,7 @@
       <c r="G149" s="12"/>
       <c r="H149" s="10"/>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" ht="12.75">
       <c r="A150" s="11"/>
       <c r="B150" s="10"/>
       <c r="C150" s="11"/>
@@ -2267,7 +2270,7 @@
       <c r="G150" s="12"/>
       <c r="H150" s="10"/>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" ht="12.75">
       <c r="A151" s="11"/>
       <c r="B151" s="10"/>
       <c r="C151" s="11"/>
@@ -2277,7 +2280,7 @@
       <c r="G151" s="12"/>
       <c r="H151" s="10"/>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" ht="12.75">
       <c r="A152" s="11"/>
       <c r="B152" s="10"/>
       <c r="C152" s="11"/>
@@ -2287,7 +2290,7 @@
       <c r="G152" s="12"/>
       <c r="H152" s="10"/>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" ht="12.75">
       <c r="A153" s="11"/>
       <c r="B153" s="10"/>
       <c r="C153" s="11"/>
@@ -2297,7 +2300,7 @@
       <c r="G153" s="12"/>
       <c r="H153" s="10"/>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" ht="12.75">
       <c r="A154" s="11"/>
       <c r="B154" s="10"/>
       <c r="C154" s="11"/>
@@ -2307,7 +2310,7 @@
       <c r="G154" s="12"/>
       <c r="H154" s="10"/>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" ht="12.75">
       <c r="A155" s="11"/>
       <c r="B155" s="10"/>
       <c r="C155" s="11"/>
@@ -2317,7 +2320,7 @@
       <c r="G155" s="12"/>
       <c r="H155" s="10"/>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" ht="12.75">
       <c r="A156" s="11"/>
       <c r="B156" s="10"/>
       <c r="C156" s="11"/>
@@ -2327,7 +2330,7 @@
       <c r="G156" s="12"/>
       <c r="H156" s="10"/>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" ht="12.75">
       <c r="A157" s="11"/>
       <c r="B157" s="10"/>
       <c r="C157" s="11"/>
@@ -2337,7 +2340,7 @@
       <c r="G157" s="12"/>
       <c r="H157" s="10"/>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" ht="12.75">
       <c r="A158" s="11"/>
       <c r="B158" s="10"/>
       <c r="C158" s="11"/>
@@ -2347,7 +2350,7 @@
       <c r="G158" s="12"/>
       <c r="H158" s="10"/>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" ht="12.75">
       <c r="A159" s="11"/>
       <c r="B159" s="10"/>
       <c r="C159" s="11"/>
@@ -2357,7 +2360,7 @@
       <c r="G159" s="12"/>
       <c r="H159" s="10"/>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" ht="12.75">
       <c r="A160" s="11"/>
       <c r="B160" s="10"/>
       <c r="C160" s="11"/>
@@ -2367,7 +2370,7 @@
       <c r="G160" s="12"/>
       <c r="H160" s="10"/>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" ht="12.75">
       <c r="A161" s="11"/>
       <c r="B161" s="10"/>
       <c r="C161" s="11"/>
@@ -2377,7 +2380,7 @@
       <c r="G161" s="12"/>
       <c r="H161" s="10"/>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" ht="12.75">
       <c r="A162" s="11"/>
       <c r="B162" s="10"/>
       <c r="C162" s="11"/>
@@ -2387,7 +2390,7 @@
       <c r="G162" s="12"/>
       <c r="H162" s="10"/>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" ht="12.75">
       <c r="A163" s="11"/>
       <c r="B163" s="10"/>
       <c r="C163" s="11"/>
@@ -2397,7 +2400,7 @@
       <c r="G163" s="12"/>
       <c r="H163" s="10"/>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" ht="12.75">
       <c r="A164" s="11"/>
       <c r="B164" s="10"/>
       <c r="C164" s="11"/>
@@ -2407,7 +2410,7 @@
       <c r="G164" s="12"/>
       <c r="H164" s="10"/>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" ht="12.75">
       <c r="A165" s="11"/>
       <c r="B165" s="10"/>
       <c r="C165" s="11"/>
@@ -2417,7 +2420,7 @@
       <c r="G165" s="12"/>
       <c r="H165" s="10"/>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" ht="12.75">
       <c r="A166" s="11"/>
       <c r="B166" s="10"/>
       <c r="C166" s="11"/>
@@ -2427,7 +2430,7 @@
       <c r="G166" s="12"/>
       <c r="H166" s="10"/>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" ht="12.75">
       <c r="A167" s="11"/>
       <c r="B167" s="10"/>
       <c r="C167" s="11"/>
@@ -2437,7 +2440,7 @@
       <c r="G167" s="12"/>
       <c r="H167" s="10"/>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" ht="12.75">
       <c r="A168" s="11"/>
       <c r="B168" s="10"/>
       <c r="C168" s="11"/>
@@ -2447,7 +2450,7 @@
       <c r="G168" s="12"/>
       <c r="H168" s="10"/>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" ht="12.75">
       <c r="A169" s="11"/>
       <c r="B169" s="10"/>
       <c r="C169" s="11"/>
@@ -2457,7 +2460,7 @@
       <c r="G169" s="12"/>
       <c r="H169" s="10"/>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" ht="12.75">
       <c r="A170" s="11"/>
       <c r="B170" s="10"/>
       <c r="C170" s="11"/>
@@ -2467,7 +2470,7 @@
       <c r="G170" s="12"/>
       <c r="H170" s="10"/>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" ht="12.75">
       <c r="A171" s="11"/>
       <c r="B171" s="10"/>
       <c r="C171" s="11"/>
@@ -2477,7 +2480,7 @@
       <c r="G171" s="12"/>
       <c r="H171" s="10"/>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" ht="12.75">
       <c r="A172" s="11"/>
       <c r="B172" s="10"/>
       <c r="C172" s="11"/>
@@ -2487,7 +2490,7 @@
       <c r="G172" s="12"/>
       <c r="H172" s="10"/>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" ht="12.75">
       <c r="A173" s="11"/>
       <c r="B173" s="10"/>
       <c r="C173" s="11"/>
@@ -2497,7 +2500,7 @@
       <c r="G173" s="12"/>
       <c r="H173" s="10"/>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" ht="12.75">
       <c r="A174" s="11"/>
       <c r="B174" s="10"/>
       <c r="C174" s="11"/>
@@ -2507,7 +2510,7 @@
       <c r="G174" s="12"/>
       <c r="H174" s="10"/>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" ht="12.75">
       <c r="A175" s="11"/>
       <c r="B175" s="10"/>
       <c r="C175" s="11"/>
@@ -2517,7 +2520,7 @@
       <c r="G175" s="12"/>
       <c r="H175" s="10"/>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" ht="12.75">
       <c r="A176" s="11"/>
       <c r="B176" s="10"/>
       <c r="C176" s="11"/>
@@ -2527,7 +2530,7 @@
       <c r="G176" s="12"/>
       <c r="H176" s="10"/>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" ht="12.75">
       <c r="A177" s="11"/>
       <c r="B177" s="10"/>
       <c r="C177" s="11"/>
@@ -2537,7 +2540,7 @@
       <c r="G177" s="12"/>
       <c r="H177" s="10"/>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" ht="12.75">
       <c r="A178" s="11"/>
       <c r="B178" s="10"/>
       <c r="C178" s="11"/>
@@ -2547,7 +2550,7 @@
       <c r="G178" s="12"/>
       <c r="H178" s="10"/>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" ht="12.75">
       <c r="A179" s="11"/>
       <c r="B179" s="10"/>
       <c r="C179" s="11"/>
@@ -2557,7 +2560,7 @@
       <c r="G179" s="12"/>
       <c r="H179" s="10"/>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" ht="12.75">
       <c r="A180" s="11"/>
       <c r="B180" s="10"/>
       <c r="C180" s="11"/>
@@ -2567,7 +2570,7 @@
       <c r="G180" s="12"/>
       <c r="H180" s="10"/>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" ht="12.75">
       <c r="A181" s="11"/>
       <c r="B181" s="10"/>
       <c r="C181" s="11"/>
@@ -2577,7 +2580,7 @@
       <c r="G181" s="12"/>
       <c r="H181" s="10"/>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" ht="12.75">
       <c r="A182" s="11"/>
       <c r="B182" s="10"/>
       <c r="C182" s="11"/>
@@ -2587,7 +2590,7 @@
       <c r="G182" s="12"/>
       <c r="H182" s="10"/>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" ht="12.75">
       <c r="A183" s="11"/>
       <c r="B183" s="10"/>
       <c r="C183" s="11"/>
@@ -2597,7 +2600,7 @@
       <c r="G183" s="12"/>
       <c r="H183" s="10"/>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" ht="12.75">
       <c r="A184" s="11"/>
       <c r="B184" s="10"/>
       <c r="C184" s="11"/>
@@ -2607,7 +2610,7 @@
       <c r="G184" s="12"/>
       <c r="H184" s="10"/>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" ht="12.75">
       <c r="A185" s="11"/>
       <c r="B185" s="10"/>
       <c r="C185" s="11"/>
@@ -2617,7 +2620,7 @@
       <c r="G185" s="12"/>
       <c r="H185" s="10"/>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" ht="12.75">
       <c r="A186" s="11"/>
       <c r="B186" s="10"/>
       <c r="C186" s="11"/>
@@ -2627,7 +2630,7 @@
       <c r="G186" s="12"/>
       <c r="H186" s="10"/>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" ht="12.75">
       <c r="A187" s="11"/>
       <c r="B187" s="10"/>
       <c r="C187" s="11"/>
@@ -2637,7 +2640,7 @@
       <c r="G187" s="12"/>
       <c r="H187" s="10"/>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" ht="12.75">
       <c r="A188" s="11"/>
       <c r="B188" s="10"/>
       <c r="C188" s="11"/>
@@ -2647,7 +2650,7 @@
       <c r="G188" s="12"/>
       <c r="H188" s="10"/>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" ht="12.75">
       <c r="A189" s="11"/>
       <c r="B189" s="10"/>
       <c r="C189" s="11"/>
@@ -2657,7 +2660,7 @@
       <c r="G189" s="12"/>
       <c r="H189" s="10"/>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" ht="12.75">
       <c r="A190" s="11"/>
       <c r="B190" s="10"/>
       <c r="C190" s="11"/>
@@ -2667,7 +2670,7 @@
       <c r="G190" s="12"/>
       <c r="H190" s="10"/>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" ht="12.75">
       <c r="A191" s="11"/>
       <c r="B191" s="10"/>
       <c r="C191" s="11"/>
@@ -2677,7 +2680,7 @@
       <c r="G191" s="12"/>
       <c r="H191" s="10"/>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" ht="12.75">
       <c r="A192" s="11"/>
       <c r="B192" s="10"/>
       <c r="C192" s="11"/>
@@ -2687,7 +2690,7 @@
       <c r="G192" s="12"/>
       <c r="H192" s="10"/>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" ht="12.75">
       <c r="A193" s="11"/>
       <c r="B193" s="10"/>
       <c r="C193" s="11"/>
@@ -2697,7 +2700,7 @@
       <c r="G193" s="12"/>
       <c r="H193" s="10"/>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" ht="12.75">
       <c r="A194" s="11"/>
       <c r="B194" s="10"/>
       <c r="C194" s="11"/>
@@ -2707,7 +2710,7 @@
       <c r="G194" s="12"/>
       <c r="H194" s="10"/>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" ht="12.75">
       <c r="A195" s="11"/>
       <c r="B195" s="10"/>
       <c r="C195" s="11"/>
@@ -2717,7 +2720,7 @@
       <c r="G195" s="12"/>
       <c r="H195" s="10"/>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" ht="12.75">
       <c r="A196" s="11"/>
       <c r="B196" s="10"/>
       <c r="C196" s="11"/>
@@ -2727,7 +2730,7 @@
       <c r="G196" s="12"/>
       <c r="H196" s="10"/>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" ht="12.75">
       <c r="A197" s="11"/>
       <c r="B197" s="10"/>
       <c r="C197" s="11"/>
@@ -2737,7 +2740,7 @@
       <c r="G197" s="12"/>
       <c r="H197" s="10"/>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" ht="12.75">
       <c r="A198" s="11"/>
       <c r="B198" s="10"/>
       <c r="C198" s="11"/>
@@ -2747,7 +2750,7 @@
       <c r="G198" s="12"/>
       <c r="H198" s="10"/>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" ht="12.75">
       <c r="A199" s="11"/>
       <c r="B199" s="10"/>
       <c r="C199" s="11"/>
@@ -2757,7 +2760,7 @@
       <c r="G199" s="12"/>
       <c r="H199" s="10"/>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" ht="12.75">
       <c r="A200" s="11"/>
       <c r="B200" s="10"/>
       <c r="C200" s="11"/>
@@ -2767,7 +2770,7 @@
       <c r="G200" s="12"/>
       <c r="H200" s="10"/>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" ht="12.75">
       <c r="A201" s="11"/>
       <c r="B201" s="10"/>
       <c r="C201" s="11"/>
@@ -2777,7 +2780,7 @@
       <c r="G201" s="12"/>
       <c r="H201" s="10"/>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" ht="12.75">
       <c r="A202" s="11"/>
       <c r="B202" s="10"/>
       <c r="C202" s="11"/>
@@ -2787,7 +2790,7 @@
       <c r="G202" s="12"/>
       <c r="H202" s="10"/>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" ht="12.75">
       <c r="A203" s="11"/>
       <c r="B203" s="10"/>
       <c r="C203" s="11"/>
@@ -2797,7 +2800,7 @@
       <c r="G203" s="12"/>
       <c r="H203" s="10"/>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" ht="12.75">
       <c r="A204" s="11"/>
       <c r="B204" s="10"/>
       <c r="C204" s="11"/>
@@ -2807,7 +2810,7 @@
       <c r="G204" s="12"/>
       <c r="H204" s="10"/>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" ht="12.75">
       <c r="A205" s="11"/>
       <c r="B205" s="10"/>
       <c r="C205" s="11"/>
@@ -2817,7 +2820,7 @@
       <c r="G205" s="12"/>
       <c r="H205" s="10"/>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" ht="12.75">
       <c r="A206" s="11"/>
       <c r="B206" s="10"/>
       <c r="C206" s="11"/>
@@ -2827,7 +2830,7 @@
       <c r="G206" s="12"/>
       <c r="H206" s="10"/>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" ht="12.75">
       <c r="A207" s="11"/>
       <c r="B207" s="10"/>
       <c r="C207" s="11"/>
@@ -2837,7 +2840,7 @@
       <c r="G207" s="12"/>
       <c r="H207" s="10"/>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" ht="12.75">
       <c r="A208" s="11"/>
       <c r="B208" s="10"/>
       <c r="C208" s="11"/>
@@ -2847,7 +2850,7 @@
       <c r="G208" s="12"/>
       <c r="H208" s="10"/>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" ht="12.75">
       <c r="A209" s="11"/>
       <c r="B209" s="10"/>
       <c r="C209" s="11"/>
@@ -2857,7 +2860,7 @@
       <c r="G209" s="12"/>
       <c r="H209" s="10"/>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" ht="12.75">
       <c r="A210" s="11"/>
       <c r="B210" s="10"/>
       <c r="C210" s="11"/>
@@ -2867,7 +2870,7 @@
       <c r="G210" s="12"/>
       <c r="H210" s="10"/>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" ht="12.75">
       <c r="A211" s="11"/>
       <c r="B211" s="10"/>
       <c r="C211" s="11"/>
@@ -2877,7 +2880,7 @@
       <c r="G211" s="12"/>
       <c r="H211" s="10"/>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" ht="12.75">
       <c r="A212" s="11"/>
       <c r="B212" s="10"/>
       <c r="C212" s="11"/>
@@ -2887,7 +2890,7 @@
       <c r="G212" s="12"/>
       <c r="H212" s="10"/>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" ht="12.75">
       <c r="A213" s="11"/>
       <c r="B213" s="10"/>
       <c r="C213" s="11"/>
@@ -2897,7 +2900,7 @@
       <c r="G213" s="12"/>
       <c r="H213" s="10"/>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" ht="12.75">
       <c r="A214" s="11"/>
       <c r="B214" s="10"/>
       <c r="C214" s="11"/>
@@ -2907,7 +2910,7 @@
       <c r="G214" s="12"/>
       <c r="H214" s="10"/>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" ht="12.75">
       <c r="A215" s="11"/>
       <c r="B215" s="10"/>
       <c r="C215" s="11"/>
@@ -2917,7 +2920,7 @@
       <c r="G215" s="12"/>
       <c r="H215" s="10"/>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" ht="12.75">
       <c r="A216" s="11"/>
       <c r="B216" s="10"/>
       <c r="C216" s="11"/>
@@ -2927,7 +2930,7 @@
       <c r="G216" s="12"/>
       <c r="H216" s="10"/>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" ht="12.75">
       <c r="A217" s="11"/>
       <c r="B217" s="10"/>
       <c r="C217" s="11"/>
@@ -2937,7 +2940,7 @@
       <c r="G217" s="12"/>
       <c r="H217" s="10"/>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" ht="12.75">
       <c r="A218" s="11"/>
       <c r="B218" s="10"/>
       <c r="C218" s="11"/>
@@ -2947,7 +2950,7 @@
       <c r="G218" s="12"/>
       <c r="H218" s="10"/>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" ht="12.75">
       <c r="A219" s="11"/>
       <c r="B219" s="10"/>
       <c r="C219" s="11"/>
@@ -2957,7 +2960,7 @@
       <c r="G219" s="12"/>
       <c r="H219" s="10"/>
     </row>
-    <row r="220" spans="1:8">
+    <row r="220" spans="1:8" ht="12.75">
       <c r="A220" s="11"/>
       <c r="B220" s="10"/>
       <c r="C220" s="11"/>
@@ -2967,7 +2970,7 @@
       <c r="G220" s="12"/>
       <c r="H220" s="10"/>
     </row>
-    <row r="221" spans="1:8">
+    <row r="221" spans="1:8" ht="12.75">
       <c r="A221" s="11"/>
       <c r="B221" s="10"/>
       <c r="C221" s="11"/>
@@ -2977,7 +2980,7 @@
       <c r="G221" s="12"/>
       <c r="H221" s="10"/>
     </row>
-    <row r="222" spans="1:8">
+    <row r="222" spans="1:8" ht="12.75">
       <c r="A222" s="11"/>
       <c r="B222" s="10"/>
       <c r="C222" s="11"/>
@@ -2987,7 +2990,7 @@
       <c r="G222" s="12"/>
       <c r="H222" s="10"/>
     </row>
-    <row r="223" spans="1:8">
+    <row r="223" spans="1:8" ht="12.75">
       <c r="A223" s="11"/>
       <c r="B223" s="10"/>
       <c r="C223" s="11"/>
@@ -2997,7 +3000,7 @@
       <c r="G223" s="12"/>
       <c r="H223" s="10"/>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" ht="12.75">
       <c r="A224" s="11"/>
       <c r="B224" s="10"/>
       <c r="C224" s="11"/>
@@ -3007,7 +3010,7 @@
       <c r="G224" s="12"/>
       <c r="H224" s="10"/>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:8" ht="12.75">
       <c r="A225" s="11"/>
       <c r="B225" s="10"/>
       <c r="C225" s="11"/>
@@ -3017,7 +3020,7 @@
       <c r="G225" s="12"/>
       <c r="H225" s="10"/>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:8" ht="12.75">
       <c r="A226" s="11"/>
       <c r="B226" s="10"/>
       <c r="C226" s="11"/>
@@ -3027,7 +3030,7 @@
       <c r="G226" s="12"/>
       <c r="H226" s="10"/>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" ht="12.75">
       <c r="A227" s="11"/>
       <c r="B227" s="10"/>
       <c r="C227" s="11"/>
@@ -3037,7 +3040,7 @@
       <c r="G227" s="12"/>
       <c r="H227" s="10"/>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" ht="12.75">
       <c r="A228" s="11"/>
       <c r="B228" s="10"/>
       <c r="C228" s="11"/>
@@ -3047,7 +3050,7 @@
       <c r="G228" s="12"/>
       <c r="H228" s="10"/>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:8" ht="12.75">
       <c r="A229" s="11"/>
       <c r="B229" s="10"/>
       <c r="C229" s="11"/>
@@ -3057,7 +3060,7 @@
       <c r="G229" s="12"/>
       <c r="H229" s="10"/>
     </row>
-    <row r="230" spans="1:8">
+    <row r="230" spans="1:8" ht="12.75">
       <c r="A230" s="11"/>
       <c r="B230" s="10"/>
       <c r="C230" s="11"/>
@@ -3067,7 +3070,7 @@
       <c r="G230" s="12"/>
       <c r="H230" s="10"/>
     </row>
-    <row r="231" spans="1:8">
+    <row r="231" spans="1:8" ht="12.75">
       <c r="A231" s="11"/>
       <c r="B231" s="10"/>
       <c r="C231" s="11"/>
@@ -3077,7 +3080,7 @@
       <c r="G231" s="12"/>
       <c r="H231" s="10"/>
     </row>
-    <row r="232" spans="1:8">
+    <row r="232" spans="1:8" ht="12.75">
       <c r="A232" s="11"/>
       <c r="B232" s="10"/>
       <c r="C232" s="11"/>
@@ -3087,7 +3090,7 @@
       <c r="G232" s="12"/>
       <c r="H232" s="10"/>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" ht="12.75">
       <c r="A233" s="11"/>
       <c r="B233" s="10"/>
       <c r="C233" s="11"/>
@@ -3097,7 +3100,7 @@
       <c r="G233" s="12"/>
       <c r="H233" s="10"/>
     </row>
-    <row r="234" spans="1:8">
+    <row r="234" spans="1:8" ht="12.75">
       <c r="A234" s="11"/>
       <c r="B234" s="10"/>
       <c r="C234" s="11"/>
@@ -3107,7 +3110,7 @@
       <c r="G234" s="12"/>
       <c r="H234" s="10"/>
     </row>
-    <row r="235" spans="1:8">
+    <row r="235" spans="1:8" ht="12.75">
       <c r="A235" s="11"/>
       <c r="B235" s="10"/>
       <c r="C235" s="11"/>
@@ -3117,7 +3120,7 @@
       <c r="G235" s="12"/>
       <c r="H235" s="10"/>
     </row>
-    <row r="236" spans="1:8">
+    <row r="236" spans="1:8" ht="12.75">
       <c r="A236" s="11"/>
       <c r="B236" s="10"/>
       <c r="C236" s="11"/>
@@ -3127,7 +3130,7 @@
       <c r="G236" s="12"/>
       <c r="H236" s="10"/>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:8" ht="12.75">
       <c r="A237" s="11"/>
       <c r="B237" s="10"/>
       <c r="C237" s="11"/>
@@ -3137,7 +3140,7 @@
       <c r="G237" s="12"/>
       <c r="H237" s="10"/>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:8" ht="12.75">
       <c r="A238" s="11"/>
       <c r="B238" s="10"/>
       <c r="C238" s="11"/>
@@ -3147,7 +3150,7 @@
       <c r="G238" s="12"/>
       <c r="H238" s="10"/>
     </row>
-    <row r="239" spans="1:8">
+    <row r="239" spans="1:8" ht="12.75">
       <c r="A239" s="11"/>
       <c r="B239" s="10"/>
       <c r="C239" s="11"/>
@@ -3157,7 +3160,7 @@
       <c r="G239" s="12"/>
       <c r="H239" s="10"/>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:8" ht="12.75">
       <c r="A240" s="11"/>
       <c r="B240" s="10"/>
       <c r="C240" s="11"/>
@@ -3167,7 +3170,7 @@
       <c r="G240" s="12"/>
       <c r="H240" s="10"/>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" ht="12.75">
       <c r="A241" s="11"/>
       <c r="B241" s="10"/>
       <c r="C241" s="11"/>
@@ -3177,7 +3180,7 @@
       <c r="G241" s="12"/>
       <c r="H241" s="10"/>
     </row>
-    <row r="242" spans="1:8">
+    <row r="242" spans="1:8" ht="12.75">
       <c r="A242" s="11"/>
       <c r="B242" s="10"/>
       <c r="C242" s="11"/>
@@ -3187,7 +3190,7 @@
       <c r="G242" s="12"/>
       <c r="H242" s="10"/>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" ht="12.75">
       <c r="A243" s="11"/>
       <c r="B243" s="10"/>
       <c r="C243" s="11"/>
@@ -3197,7 +3200,7 @@
       <c r="G243" s="12"/>
       <c r="H243" s="10"/>
     </row>
-    <row r="244" spans="1:8">
+    <row r="244" spans="1:8" ht="12.75">
       <c r="A244" s="11"/>
       <c r="B244" s="10"/>
       <c r="C244" s="11"/>
@@ -3207,7 +3210,7 @@
       <c r="G244" s="12"/>
       <c r="H244" s="10"/>
     </row>
-    <row r="245" spans="1:8">
+    <row r="245" spans="1:8" ht="12.75">
       <c r="A245" s="11"/>
       <c r="B245" s="10"/>
       <c r="C245" s="11"/>
@@ -3217,7 +3220,7 @@
       <c r="G245" s="12"/>
       <c r="H245" s="10"/>
     </row>
-    <row r="246" spans="1:8">
+    <row r="246" spans="1:8" ht="12.75">
       <c r="A246" s="11"/>
       <c r="B246" s="10"/>
       <c r="C246" s="11"/>
@@ -3227,7 +3230,7 @@
       <c r="G246" s="12"/>
       <c r="H246" s="10"/>
     </row>
-    <row r="247" spans="1:8">
+    <row r="247" spans="1:8" ht="12.75">
       <c r="A247" s="11"/>
       <c r="B247" s="10"/>
       <c r="C247" s="11"/>
@@ -3237,7 +3240,7 @@
       <c r="G247" s="12"/>
       <c r="H247" s="10"/>
     </row>
-    <row r="248" spans="1:8">
+    <row r="248" spans="1:8" ht="12.75">
       <c r="A248" s="11"/>
       <c r="B248" s="10"/>
       <c r="C248" s="11"/>
@@ -3247,7 +3250,7 @@
       <c r="G248" s="12"/>
       <c r="H248" s="10"/>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" ht="12.75">
       <c r="A249" s="11"/>
       <c r="B249" s="10"/>
       <c r="C249" s="11"/>
@@ -3257,7 +3260,7 @@
       <c r="G249" s="12"/>
       <c r="H249" s="10"/>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" ht="12.75">
       <c r="A250" s="11"/>
       <c r="B250" s="10"/>
       <c r="C250" s="11"/>
@@ -3267,7 +3270,7 @@
       <c r="G250" s="12"/>
       <c r="H250" s="10"/>
     </row>
-    <row r="251" spans="1:8">
+    <row r="251" spans="1:8" ht="12.75">
       <c r="A251" s="11"/>
       <c r="B251" s="10"/>
       <c r="C251" s="11"/>
@@ -3277,7 +3280,7 @@
       <c r="G251" s="12"/>
       <c r="H251" s="10"/>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" ht="12.75">
       <c r="A252" s="11"/>
       <c r="B252" s="10"/>
       <c r="C252" s="11"/>
@@ -3287,7 +3290,7 @@
       <c r="G252" s="12"/>
       <c r="H252" s="10"/>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" ht="12.75">
       <c r="A253" s="11"/>
       <c r="B253" s="10"/>
       <c r="C253" s="11"/>
@@ -3297,7 +3300,7 @@
       <c r="G253" s="12"/>
       <c r="H253" s="10"/>
     </row>
-    <row r="254" spans="1:8">
+    <row r="254" spans="1:8" ht="12.75">
       <c r="A254" s="11"/>
       <c r="B254" s="10"/>
       <c r="C254" s="11"/>
@@ -3307,7 +3310,7 @@
       <c r="G254" s="12"/>
       <c r="H254" s="10"/>
     </row>
-    <row r="255" spans="1:8">
+    <row r="255" spans="1:8" ht="12.75">
       <c r="A255" s="11"/>
       <c r="B255" s="10"/>
       <c r="C255" s="11"/>
@@ -3317,7 +3320,7 @@
       <c r="G255" s="12"/>
       <c r="H255" s="10"/>
     </row>
-    <row r="256" spans="1:8">
+    <row r="256" spans="1:8" ht="12.75">
       <c r="A256" s="11"/>
       <c r="B256" s="10"/>
       <c r="C256" s="11"/>
@@ -3327,7 +3330,7 @@
       <c r="G256" s="12"/>
       <c r="H256" s="10"/>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" ht="12.75">
       <c r="A257" s="11"/>
       <c r="B257" s="10"/>
       <c r="C257" s="11"/>
@@ -3337,7 +3340,7 @@
       <c r="G257" s="12"/>
       <c r="H257" s="10"/>
     </row>
-    <row r="258" spans="1:8">
+    <row r="258" spans="1:8" ht="12.75">
       <c r="A258" s="11"/>
       <c r="B258" s="10"/>
       <c r="C258" s="11"/>
@@ -3347,7 +3350,7 @@
       <c r="G258" s="12"/>
       <c r="H258" s="10"/>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" ht="12.75">
       <c r="A259" s="11"/>
       <c r="B259" s="10"/>
       <c r="C259" s="11"/>
@@ -3357,7 +3360,7 @@
       <c r="G259" s="12"/>
       <c r="H259" s="10"/>
     </row>
-    <row r="260" spans="1:8">
+    <row r="260" spans="1:8" ht="12.75">
       <c r="A260" s="11"/>
       <c r="B260" s="10"/>
       <c r="C260" s="11"/>
@@ -3367,7 +3370,7 @@
       <c r="G260" s="12"/>
       <c r="H260" s="10"/>
     </row>
-    <row r="261" spans="1:8">
+    <row r="261" spans="1:8" ht="12.75">
       <c r="A261" s="11"/>
       <c r="B261" s="10"/>
       <c r="C261" s="11"/>
@@ -3377,7 +3380,7 @@
       <c r="G261" s="12"/>
       <c r="H261" s="10"/>
     </row>
-    <row r="262" spans="1:8">
+    <row r="262" spans="1:8" ht="12.75">
       <c r="A262" s="11"/>
       <c r="B262" s="10"/>
       <c r="C262" s="11"/>
@@ -3387,7 +3390,7 @@
       <c r="G262" s="12"/>
       <c r="H262" s="10"/>
     </row>
-    <row r="263" spans="1:8">
+    <row r="263" spans="1:8" ht="12.75">
       <c r="A263" s="11"/>
       <c r="B263" s="10"/>
       <c r="C263" s="11"/>
@@ -3397,7 +3400,7 @@
       <c r="G263" s="12"/>
       <c r="H263" s="10"/>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" ht="12.75">
       <c r="A264" s="11"/>
       <c r="B264" s="10"/>
       <c r="C264" s="11"/>
@@ -3407,7 +3410,7 @@
       <c r="G264" s="12"/>
       <c r="H264" s="10"/>
     </row>
-    <row r="265" spans="1:8">
+    <row r="265" spans="1:8" ht="12.75">
       <c r="A265" s="11"/>
       <c r="B265" s="10"/>
       <c r="C265" s="11"/>
@@ -3417,7 +3420,7 @@
       <c r="G265" s="12"/>
       <c r="H265" s="10"/>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" ht="12.75">
       <c r="A266" s="11"/>
       <c r="B266" s="10"/>
       <c r="C266" s="11"/>
@@ -3427,7 +3430,7 @@
       <c r="G266" s="12"/>
       <c r="H266" s="10"/>
     </row>
-    <row r="267" spans="1:8">
+    <row r="267" spans="1:8" ht="12.75">
       <c r="A267" s="11"/>
       <c r="B267" s="10"/>
       <c r="C267" s="11"/>
@@ -3437,7 +3440,7 @@
       <c r="G267" s="12"/>
       <c r="H267" s="10"/>
     </row>
-    <row r="268" spans="1:8">
+    <row r="268" spans="1:8" ht="12.75">
       <c r="A268" s="11"/>
       <c r="B268" s="10"/>
       <c r="C268" s="11"/>
@@ -3447,7 +3450,7 @@
       <c r="G268" s="12"/>
       <c r="H268" s="10"/>
     </row>
-    <row r="269" spans="1:8">
+    <row r="269" spans="1:8" ht="12.75">
       <c r="A269" s="11"/>
       <c r="B269" s="10"/>
       <c r="C269" s="11"/>
@@ -3457,7 +3460,7 @@
       <c r="G269" s="12"/>
       <c r="H269" s="10"/>
     </row>
-    <row r="270" spans="1:8">
+    <row r="270" spans="1:8" ht="12.75">
       <c r="A270" s="11"/>
       <c r="B270" s="10"/>
       <c r="C270" s="11"/>
@@ -3467,7 +3470,7 @@
       <c r="G270" s="12"/>
       <c r="H270" s="10"/>
     </row>
-    <row r="271" spans="1:8">
+    <row r="271" spans="1:8" ht="12.75">
       <c r="A271" s="11"/>
       <c r="B271" s="10"/>
       <c r="C271" s="11"/>
@@ -3477,7 +3480,7 @@
       <c r="G271" s="12"/>
       <c r="H271" s="10"/>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" ht="12.75">
       <c r="A272" s="11"/>
       <c r="B272" s="10"/>
       <c r="C272" s="11"/>
@@ -3487,7 +3490,7 @@
       <c r="G272" s="12"/>
       <c r="H272" s="10"/>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:8" ht="12.75">
       <c r="A273" s="11"/>
       <c r="B273" s="10"/>
       <c r="C273" s="11"/>
@@ -3497,7 +3500,7 @@
       <c r="G273" s="12"/>
       <c r="H273" s="10"/>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:8" ht="12.75">
       <c r="A274" s="11"/>
       <c r="B274" s="10"/>
       <c r="C274" s="11"/>
@@ -3507,7 +3510,7 @@
       <c r="G274" s="12"/>
       <c r="H274" s="10"/>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" ht="12.75">
       <c r="A275" s="11"/>
       <c r="B275" s="10"/>
       <c r="C275" s="11"/>
@@ -3517,7 +3520,7 @@
       <c r="G275" s="12"/>
       <c r="H275" s="10"/>
     </row>
-    <row r="276" spans="1:8">
+    <row r="276" spans="1:8" ht="12.75">
       <c r="A276" s="11"/>
       <c r="B276" s="10"/>
       <c r="C276" s="11"/>
@@ -3527,7 +3530,7 @@
       <c r="G276" s="12"/>
       <c r="H276" s="10"/>
     </row>
-    <row r="277" spans="1:8">
+    <row r="277" spans="1:8" ht="12.75">
       <c r="A277" s="11"/>
       <c r="B277" s="10"/>
       <c r="C277" s="11"/>
@@ -3537,7 +3540,7 @@
       <c r="G277" s="12"/>
       <c r="H277" s="10"/>
     </row>
-    <row r="278" spans="1:8">
+    <row r="278" spans="1:8" ht="12.75">
       <c r="A278" s="11"/>
       <c r="B278" s="10"/>
       <c r="C278" s="11"/>
@@ -3547,7 +3550,7 @@
       <c r="G278" s="12"/>
       <c r="H278" s="10"/>
     </row>
-    <row r="279" spans="1:8">
+    <row r="279" spans="1:8" ht="12.75">
       <c r="A279" s="11"/>
       <c r="B279" s="10"/>
       <c r="C279" s="11"/>
@@ -3557,7 +3560,7 @@
       <c r="G279" s="12"/>
       <c r="H279" s="10"/>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" ht="12.75">
       <c r="A280" s="11"/>
       <c r="B280" s="10"/>
       <c r="C280" s="11"/>
@@ -3567,7 +3570,7 @@
       <c r="G280" s="12"/>
       <c r="H280" s="10"/>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" ht="12.75">
       <c r="A281" s="11"/>
       <c r="B281" s="10"/>
       <c r="C281" s="11"/>
@@ -3577,7 +3580,7 @@
       <c r="G281" s="12"/>
       <c r="H281" s="10"/>
     </row>
-    <row r="282" spans="1:8">
+    <row r="282" spans="1:8" ht="12.75">
       <c r="A282" s="11"/>
       <c r="B282" s="10"/>
       <c r="C282" s="11"/>
@@ -3587,7 +3590,7 @@
       <c r="G282" s="12"/>
       <c r="H282" s="10"/>
     </row>
-    <row r="283" spans="1:8">
+    <row r="283" spans="1:8" ht="12.75">
       <c r="A283" s="11"/>
       <c r="B283" s="10"/>
       <c r="C283" s="11"/>
@@ -3597,7 +3600,7 @@
       <c r="G283" s="12"/>
       <c r="H283" s="10"/>
     </row>
-    <row r="284" spans="1:8">
+    <row r="284" spans="1:8" ht="12.75">
       <c r="A284" s="11"/>
       <c r="B284" s="10"/>
       <c r="C284" s="11"/>
@@ -3607,7 +3610,7 @@
       <c r="G284" s="12"/>
       <c r="H284" s="10"/>
     </row>
-    <row r="285" spans="1:8">
+    <row r="285" spans="1:8" ht="12.75">
       <c r="A285" s="11"/>
       <c r="B285" s="10"/>
       <c r="C285" s="11"/>
@@ -3617,7 +3620,7 @@
       <c r="G285" s="12"/>
       <c r="H285" s="10"/>
     </row>
-    <row r="286" spans="1:8">
+    <row r="286" spans="1:8" ht="12.75">
       <c r="A286" s="11"/>
       <c r="B286" s="10"/>
       <c r="C286" s="11"/>
@@ -3627,7 +3630,7 @@
       <c r="G286" s="12"/>
       <c r="H286" s="10"/>
     </row>
-    <row r="287" spans="1:8">
+    <row r="287" spans="1:8" ht="12.75">
       <c r="A287" s="11"/>
       <c r="B287" s="10"/>
       <c r="C287" s="11"/>
@@ -3637,7 +3640,7 @@
       <c r="G287" s="12"/>
       <c r="H287" s="10"/>
     </row>
-    <row r="288" spans="1:8">
+    <row r="288" spans="1:8" ht="12.75">
       <c r="A288" s="11"/>
       <c r="B288" s="10"/>
       <c r="C288" s="11"/>
@@ -3647,7 +3650,7 @@
       <c r="G288" s="12"/>
       <c r="H288" s="10"/>
     </row>
-    <row r="289" spans="1:8">
+    <row r="289" spans="1:8" ht="12.75">
       <c r="A289" s="11"/>
       <c r="B289" s="10"/>
       <c r="C289" s="11"/>
@@ -3657,7 +3660,7 @@
       <c r="G289" s="12"/>
       <c r="H289" s="10"/>
     </row>
-    <row r="290" spans="1:8">
+    <row r="290" spans="1:8" ht="12.75">
       <c r="A290" s="11"/>
       <c r="B290" s="10"/>
       <c r="C290" s="11"/>
@@ -3667,7 +3670,7 @@
       <c r="G290" s="12"/>
       <c r="H290" s="10"/>
     </row>
-    <row r="291" spans="1:8">
+    <row r="291" spans="1:8" ht="12.75">
       <c r="A291" s="11"/>
       <c r="B291" s="10"/>
       <c r="C291" s="11"/>
@@ -3677,7 +3680,7 @@
       <c r="G291" s="12"/>
       <c r="H291" s="10"/>
     </row>
-    <row r="292" spans="1:8">
+    <row r="292" spans="1:8" ht="12.75">
       <c r="A292" s="11"/>
       <c r="B292" s="10"/>
       <c r="C292" s="11"/>
@@ -3687,7 +3690,7 @@
       <c r="G292" s="12"/>
       <c r="H292" s="10"/>
     </row>
-    <row r="293" spans="1:8">
+    <row r="293" spans="1:8" ht="12.75">
       <c r="A293" s="11"/>
       <c r="B293" s="10"/>
       <c r="C293" s="11"/>
@@ -3697,7 +3700,7 @@
       <c r="G293" s="12"/>
       <c r="H293" s="10"/>
     </row>
-    <row r="294" spans="1:8">
+    <row r="294" spans="1:8" ht="12.75">
       <c r="A294" s="11"/>
       <c r="B294" s="10"/>
       <c r="C294" s="11"/>
@@ -3707,7 +3710,7 @@
       <c r="G294" s="12"/>
       <c r="H294" s="10"/>
     </row>
-    <row r="295" spans="1:8">
+    <row r="295" spans="1:8" ht="12.75">
       <c r="A295" s="11"/>
       <c r="B295" s="10"/>
       <c r="C295" s="11"/>
@@ -3717,7 +3720,7 @@
       <c r="G295" s="12"/>
       <c r="H295" s="10"/>
     </row>
-    <row r="296" spans="1:8">
+    <row r="296" spans="1:8" ht="12.75">
       <c r="A296" s="11"/>
       <c r="B296" s="10"/>
       <c r="C296" s="11"/>
@@ -3727,7 +3730,7 @@
       <c r="G296" s="12"/>
       <c r="H296" s="10"/>
     </row>
-    <row r="297" spans="1:8">
+    <row r="297" spans="1:8" ht="12.75">
       <c r="A297" s="11"/>
       <c r="B297" s="10"/>
       <c r="C297" s="11"/>
@@ -3737,7 +3740,7 @@
       <c r="G297" s="12"/>
       <c r="H297" s="10"/>
     </row>
-    <row r="298" spans="1:8">
+    <row r="298" spans="1:8" ht="12.75">
       <c r="A298" s="11"/>
       <c r="B298" s="10"/>
       <c r="C298" s="11"/>
@@ -3747,7 +3750,7 @@
       <c r="G298" s="12"/>
       <c r="H298" s="10"/>
     </row>
-    <row r="299" spans="1:8">
+    <row r="299" spans="1:8" ht="12.75">
       <c r="A299" s="11"/>
       <c r="B299" s="10"/>
       <c r="C299" s="11"/>
@@ -3757,7 +3760,7 @@
       <c r="G299" s="12"/>
       <c r="H299" s="10"/>
     </row>
-    <row r="300" spans="1:8">
+    <row r="300" spans="1:8" ht="12.75">
       <c r="A300" s="11"/>
       <c r="B300" s="10"/>
       <c r="C300" s="11"/>
@@ -3767,7 +3770,7 @@
       <c r="G300" s="12"/>
       <c r="H300" s="10"/>
     </row>
-    <row r="301" spans="1:8">
+    <row r="301" spans="1:8" ht="12.75">
       <c r="A301" s="11"/>
       <c r="B301" s="10"/>
       <c r="C301" s="11"/>
@@ -3777,7 +3780,7 @@
       <c r="G301" s="12"/>
       <c r="H301" s="10"/>
     </row>
-    <row r="302" spans="1:8">
+    <row r="302" spans="1:8" ht="12.75">
       <c r="A302" s="11"/>
       <c r="B302" s="10"/>
       <c r="C302" s="11"/>
@@ -3787,7 +3790,7 @@
       <c r="G302" s="12"/>
       <c r="H302" s="10"/>
     </row>
-    <row r="303" spans="1:8">
+    <row r="303" spans="1:8" ht="12.75">
       <c r="A303" s="11"/>
       <c r="B303" s="10"/>
       <c r="C303" s="11"/>
@@ -3797,7 +3800,7 @@
       <c r="G303" s="12"/>
       <c r="H303" s="10"/>
     </row>
-    <row r="304" spans="1:8">
+    <row r="304" spans="1:8" ht="12.75">
       <c r="A304" s="11"/>
       <c r="B304" s="10"/>
       <c r="C304" s="11"/>
@@ -3807,7 +3810,7 @@
       <c r="G304" s="12"/>
       <c r="H304" s="10"/>
     </row>
-    <row r="305" spans="1:8">
+    <row r="305" spans="1:8" ht="12.75">
       <c r="A305" s="11"/>
       <c r="B305" s="10"/>
       <c r="C305" s="11"/>
@@ -3817,7 +3820,7 @@
       <c r="G305" s="12"/>
       <c r="H305" s="10"/>
     </row>
-    <row r="306" spans="1:8">
+    <row r="306" spans="1:8" ht="12.75">
       <c r="A306" s="11"/>
       <c r="B306" s="10"/>
       <c r="C306" s="11"/>
@@ -3827,7 +3830,7 @@
       <c r="G306" s="12"/>
       <c r="H306" s="10"/>
     </row>
-    <row r="307" spans="1:8">
+    <row r="307" spans="1:8" ht="12.75">
       <c r="A307" s="11"/>
       <c r="B307" s="10"/>
       <c r="C307" s="11"/>
@@ -3837,7 +3840,7 @@
       <c r="G307" s="12"/>
       <c r="H307" s="10"/>
     </row>
-    <row r="308" spans="1:8">
+    <row r="308" spans="1:8" ht="12.75">
       <c r="A308" s="11"/>
       <c r="B308" s="10"/>
       <c r="C308" s="11"/>
@@ -3847,7 +3850,7 @@
       <c r="G308" s="12"/>
       <c r="H308" s="10"/>
     </row>
-    <row r="309" spans="1:8">
+    <row r="309" spans="1:8" ht="12.75">
       <c r="A309" s="11"/>
       <c r="B309" s="10"/>
       <c r="C309" s="11"/>
@@ -3857,7 +3860,7 @@
       <c r="G309" s="12"/>
       <c r="H309" s="10"/>
     </row>
-    <row r="310" spans="1:8">
+    <row r="310" spans="1:8" ht="12.75">
       <c r="A310" s="11"/>
       <c r="B310" s="10"/>
       <c r="C310" s="11"/>
@@ -3867,7 +3870,7 @@
       <c r="G310" s="12"/>
       <c r="H310" s="10"/>
     </row>
-    <row r="311" spans="1:8">
+    <row r="311" spans="1:8" ht="12.75">
       <c r="A311" s="11"/>
       <c r="B311" s="10"/>
       <c r="C311" s="11"/>
@@ -3877,7 +3880,7 @@
       <c r="G311" s="12"/>
       <c r="H311" s="10"/>
     </row>
-    <row r="312" spans="1:8">
+    <row r="312" spans="1:8" ht="12.75">
       <c r="A312" s="11"/>
       <c r="B312" s="10"/>
       <c r="C312" s="11"/>
@@ -3887,7 +3890,7 @@
       <c r="G312" s="12"/>
       <c r="H312" s="10"/>
     </row>
-    <row r="313" spans="1:8">
+    <row r="313" spans="1:8" ht="12.75">
       <c r="A313" s="11"/>
       <c r="B313" s="10"/>
       <c r="C313" s="11"/>
@@ -3897,7 +3900,7 @@
       <c r="G313" s="12"/>
       <c r="H313" s="10"/>
     </row>
-    <row r="314" spans="1:8">
+    <row r="314" spans="1:8" ht="12.75">
       <c r="A314" s="11"/>
       <c r="B314" s="10"/>
       <c r="C314" s="11"/>
@@ -3907,7 +3910,7 @@
       <c r="G314" s="12"/>
       <c r="H314" s="10"/>
     </row>
-    <row r="315" spans="1:8">
+    <row r="315" spans="1:8" ht="12.75">
       <c r="A315" s="11"/>
       <c r="B315" s="10"/>
       <c r="C315" s="11"/>
@@ -3917,7 +3920,7 @@
       <c r="G315" s="12"/>
       <c r="H315" s="10"/>
     </row>
-    <row r="316" spans="1:8">
+    <row r="316" spans="1:8" ht="12.75">
       <c r="A316" s="11"/>
       <c r="B316" s="10"/>
       <c r="C316" s="11"/>
@@ -3927,7 +3930,7 @@
       <c r="G316" s="12"/>
       <c r="H316" s="10"/>
     </row>
-    <row r="317" spans="1:8">
+    <row r="317" spans="1:8" ht="12.75">
       <c r="A317" s="11"/>
       <c r="B317" s="10"/>
       <c r="C317" s="11"/>
@@ -3937,7 +3940,7 @@
       <c r="G317" s="12"/>
       <c r="H317" s="10"/>
     </row>
-    <row r="318" spans="1:8">
+    <row r="318" spans="1:8" ht="12.75">
       <c r="A318" s="11"/>
       <c r="B318" s="10"/>
       <c r="C318" s="11"/>
@@ -3947,7 +3950,7 @@
       <c r="G318" s="12"/>
       <c r="H318" s="10"/>
     </row>
-    <row r="319" spans="1:8">
+    <row r="319" spans="1:8" ht="12.75">
       <c r="A319" s="11"/>
       <c r="B319" s="10"/>
       <c r="C319" s="11"/>
@@ -3957,7 +3960,7 @@
       <c r="G319" s="12"/>
       <c r="H319" s="10"/>
     </row>
-    <row r="320" spans="1:8">
+    <row r="320" spans="1:8" ht="12.75">
       <c r="A320" s="11"/>
       <c r="B320" s="10"/>
       <c r="C320" s="11"/>
@@ -3967,7 +3970,7 @@
       <c r="G320" s="12"/>
       <c r="H320" s="10"/>
     </row>
-    <row r="321" spans="1:8">
+    <row r="321" spans="1:8" ht="12.75">
       <c r="A321" s="11"/>
       <c r="B321" s="10"/>
       <c r="C321" s="11"/>
@@ -3977,7 +3980,7 @@
       <c r="G321" s="12"/>
       <c r="H321" s="10"/>
     </row>
-    <row r="322" spans="1:8">
+    <row r="322" spans="1:8" ht="12.75">
       <c r="A322" s="11"/>
       <c r="B322" s="10"/>
       <c r="C322" s="11"/>
@@ -3987,7 +3990,7 @@
       <c r="G322" s="12"/>
       <c r="H322" s="10"/>
     </row>
-    <row r="323" spans="1:8">
+    <row r="323" spans="1:8" ht="12.75">
       <c r="A323" s="11"/>
       <c r="B323" s="10"/>
       <c r="C323" s="11"/>
@@ -3997,7 +4000,7 @@
       <c r="G323" s="12"/>
       <c r="H323" s="10"/>
     </row>
-    <row r="324" spans="1:8">
+    <row r="324" spans="1:8" ht="12.75">
       <c r="A324" s="11"/>
       <c r="B324" s="10"/>
       <c r="C324" s="11"/>
@@ -4007,7 +4010,7 @@
       <c r="G324" s="12"/>
       <c r="H324" s="10"/>
     </row>
-    <row r="325" spans="1:8">
+    <row r="325" spans="1:8" ht="12.75">
       <c r="A325" s="11"/>
       <c r="B325" s="10"/>
       <c r="C325" s="11"/>
@@ -4017,7 +4020,7 @@
       <c r="G325" s="12"/>
       <c r="H325" s="10"/>
     </row>
-    <row r="326" spans="1:8">
+    <row r="326" spans="1:8" ht="12.75">
       <c r="A326" s="11"/>
       <c r="B326" s="10"/>
       <c r="C326" s="11"/>
@@ -4027,7 +4030,7 @@
       <c r="G326" s="12"/>
       <c r="H326" s="10"/>
     </row>
-    <row r="327" spans="1:8">
+    <row r="327" spans="1:8" ht="12.75">
       <c r="A327" s="11"/>
       <c r="B327" s="10"/>
       <c r="C327" s="11"/>
@@ -4037,7 +4040,7 @@
       <c r="G327" s="12"/>
       <c r="H327" s="10"/>
     </row>
-    <row r="328" spans="1:8">
+    <row r="328" spans="1:8" ht="12.75">
       <c r="A328" s="11"/>
       <c r="B328" s="10"/>
       <c r="C328" s="11"/>
@@ -4047,7 +4050,7 @@
       <c r="G328" s="12"/>
       <c r="H328" s="10"/>
     </row>
-    <row r="329" spans="1:8">
+    <row r="329" spans="1:8" ht="12.75">
       <c r="A329" s="11"/>
       <c r="B329" s="10"/>
       <c r="C329" s="11"/>
@@ -4057,7 +4060,7 @@
       <c r="G329" s="12"/>
       <c r="H329" s="10"/>
     </row>
-    <row r="330" spans="1:8">
+    <row r="330" spans="1:8" ht="12.75">
       <c r="A330" s="11"/>
       <c r="B330" s="10"/>
       <c r="C330" s="11"/>
@@ -4067,7 +4070,7 @@
       <c r="G330" s="12"/>
       <c r="H330" s="10"/>
     </row>
-    <row r="331" spans="1:8">
+    <row r="331" spans="1:8" ht="12.75">
       <c r="A331" s="11"/>
       <c r="B331" s="10"/>
       <c r="C331" s="11"/>
@@ -4077,7 +4080,7 @@
       <c r="G331" s="12"/>
       <c r="H331" s="10"/>
     </row>
-    <row r="332" spans="1:8">
+    <row r="332" spans="1:8" ht="12.75">
       <c r="A332" s="11"/>
       <c r="B332" s="10"/>
       <c r="C332" s="11"/>
@@ -4087,7 +4090,7 @@
       <c r="G332" s="12"/>
       <c r="H332" s="10"/>
     </row>
-    <row r="333" spans="1:8">
+    <row r="333" spans="1:8" ht="12.75">
       <c r="A333" s="11"/>
       <c r="B333" s="10"/>
       <c r="C333" s="11"/>
@@ -4097,7 +4100,7 @@
       <c r="G333" s="12"/>
       <c r="H333" s="10"/>
     </row>
-    <row r="334" spans="1:8">
+    <row r="334" spans="1:8" ht="12.75">
       <c r="A334" s="11"/>
       <c r="B334" s="10"/>
       <c r="C334" s="11"/>
@@ -4107,7 +4110,7 @@
       <c r="G334" s="12"/>
       <c r="H334" s="10"/>
     </row>
-    <row r="335" spans="1:8">
+    <row r="335" spans="1:8" ht="12.75">
       <c r="A335" s="11"/>
       <c r="B335" s="10"/>
       <c r="C335" s="11"/>
@@ -4117,7 +4120,7 @@
       <c r="G335" s="12"/>
       <c r="H335" s="10"/>
     </row>
-    <row r="336" spans="1:8">
+    <row r="336" spans="1:8" ht="12.75">
       <c r="A336" s="11"/>
       <c r="B336" s="10"/>
       <c r="C336" s="11"/>
@@ -4127,7 +4130,7 @@
       <c r="G336" s="12"/>
       <c r="H336" s="10"/>
     </row>
-    <row r="337" spans="1:8">
+    <row r="337" spans="1:8" ht="12.75">
       <c r="A337" s="11"/>
       <c r="B337" s="10"/>
       <c r="C337" s="11"/>
@@ -4137,7 +4140,7 @@
       <c r="G337" s="12"/>
       <c r="H337" s="10"/>
     </row>
-    <row r="338" spans="1:8">
+    <row r="338" spans="1:8" ht="12.75">
       <c r="A338" s="11"/>
       <c r="B338" s="10"/>
       <c r="C338" s="11"/>
@@ -4147,7 +4150,7 @@
       <c r="G338" s="12"/>
       <c r="H338" s="10"/>
     </row>
-    <row r="339" spans="1:8">
+    <row r="339" spans="1:8" ht="12.75">
       <c r="A339" s="11"/>
       <c r="B339" s="10"/>
       <c r="C339" s="11"/>
@@ -4157,7 +4160,7 @@
       <c r="G339" s="12"/>
       <c r="H339" s="10"/>
     </row>
-    <row r="340" spans="1:8">
+    <row r="340" spans="1:8" ht="12.75">
       <c r="A340" s="11"/>
       <c r="B340" s="10"/>
       <c r="C340" s="11"/>
@@ -4167,7 +4170,7 @@
       <c r="G340" s="12"/>
       <c r="H340" s="10"/>
     </row>
-    <row r="341" spans="1:8">
+    <row r="341" spans="1:8" ht="12.75">
       <c r="A341" s="11"/>
       <c r="B341" s="10"/>
       <c r="C341" s="11"/>
@@ -4177,7 +4180,7 @@
       <c r="G341" s="12"/>
       <c r="H341" s="10"/>
     </row>
-    <row r="342" spans="1:8">
+    <row r="342" spans="1:8" ht="12.75">
       <c r="A342" s="11"/>
       <c r="B342" s="10"/>
       <c r="C342" s="11"/>
@@ -4187,7 +4190,7 @@
       <c r="G342" s="12"/>
       <c r="H342" s="10"/>
     </row>
-    <row r="343" spans="1:8">
+    <row r="343" spans="1:8" ht="12.75">
       <c r="A343" s="11"/>
       <c r="B343" s="10"/>
       <c r="C343" s="11"/>
@@ -4197,7 +4200,7 @@
       <c r="G343" s="12"/>
       <c r="H343" s="10"/>
     </row>
-    <row r="344" spans="1:8">
+    <row r="344" spans="1:8" ht="12.75">
       <c r="A344" s="11"/>
       <c r="B344" s="10"/>
       <c r="C344" s="11"/>
@@ -4207,7 +4210,7 @@
       <c r="G344" s="12"/>
       <c r="H344" s="10"/>
     </row>
-    <row r="345" spans="1:8">
+    <row r="345" spans="1:8" ht="12.75">
       <c r="A345" s="11"/>
       <c r="B345" s="10"/>
       <c r="C345" s="11"/>
@@ -4217,7 +4220,7 @@
       <c r="G345" s="12"/>
       <c r="H345" s="10"/>
     </row>
-    <row r="346" spans="1:8">
+    <row r="346" spans="1:8" ht="12.75">
       <c r="A346" s="11"/>
       <c r="B346" s="10"/>
       <c r="C346" s="11"/>
@@ -4227,7 +4230,7 @@
       <c r="G346" s="12"/>
       <c r="H346" s="10"/>
     </row>
-    <row r="347" spans="1:8">
+    <row r="347" spans="1:8" ht="12.75">
       <c r="A347" s="11"/>
       <c r="B347" s="10"/>
       <c r="C347" s="11"/>
@@ -4237,7 +4240,7 @@
       <c r="G347" s="12"/>
       <c r="H347" s="10"/>
     </row>
-    <row r="348" spans="1:8">
+    <row r="348" spans="1:8" ht="12.75">
       <c r="A348" s="11"/>
       <c r="B348" s="10"/>
       <c r="C348" s="11"/>
@@ -4247,7 +4250,7 @@
       <c r="G348" s="12"/>
       <c r="H348" s="10"/>
     </row>
-    <row r="349" spans="1:8">
+    <row r="349" spans="1:8" ht="12.75">
       <c r="A349" s="11"/>
       <c r="B349" s="10"/>
       <c r="C349" s="11"/>
@@ -4257,7 +4260,7 @@
       <c r="G349" s="12"/>
       <c r="H349" s="10"/>
     </row>
-    <row r="350" spans="1:8">
+    <row r="350" spans="1:8" ht="12.75">
       <c r="A350" s="11"/>
       <c r="B350" s="10"/>
       <c r="C350" s="11"/>
@@ -4267,7 +4270,7 @@
       <c r="G350" s="12"/>
       <c r="H350" s="10"/>
     </row>
-    <row r="351" spans="1:8">
+    <row r="351" spans="1:8" ht="12.75">
       <c r="A351" s="11"/>
       <c r="B351" s="10"/>
       <c r="C351" s="11"/>
@@ -4277,7 +4280,7 @@
       <c r="G351" s="12"/>
       <c r="H351" s="10"/>
     </row>
-    <row r="352" spans="1:8">
+    <row r="352" spans="1:8" ht="12.75">
       <c r="A352" s="11"/>
       <c r="B352" s="10"/>
       <c r="C352" s="11"/>
@@ -4287,7 +4290,7 @@
       <c r="G352" s="12"/>
       <c r="H352" s="10"/>
     </row>
-    <row r="353" spans="1:8">
+    <row r="353" spans="1:8" ht="12.75">
       <c r="A353" s="11"/>
       <c r="B353" s="10"/>
       <c r="C353" s="11"/>
@@ -4297,7 +4300,7 @@
       <c r="G353" s="12"/>
       <c r="H353" s="10"/>
     </row>
-    <row r="354" spans="1:8">
+    <row r="354" spans="1:8" ht="12.75">
       <c r="A354" s="11"/>
       <c r="B354" s="10"/>
       <c r="C354" s="11"/>
@@ -4307,7 +4310,7 @@
       <c r="G354" s="12"/>
       <c r="H354" s="10"/>
     </row>
-    <row r="355" spans="1:8">
+    <row r="355" spans="1:8" ht="12.75">
       <c r="A355" s="11"/>
       <c r="B355" s="10"/>
       <c r="C355" s="11"/>
@@ -4317,7 +4320,7 @@
       <c r="G355" s="12"/>
       <c r="H355" s="10"/>
     </row>
-    <row r="356" spans="1:8">
+    <row r="356" spans="1:8" ht="12.75">
       <c r="A356" s="11"/>
       <c r="B356" s="10"/>
       <c r="C356" s="11"/>
@@ -4327,7 +4330,7 @@
       <c r="G356" s="12"/>
       <c r="H356" s="10"/>
     </row>
-    <row r="357" spans="1:8">
+    <row r="357" spans="1:8" ht="12.75">
       <c r="A357" s="11"/>
       <c r="B357" s="10"/>
       <c r="C357" s="11"/>
@@ -4337,7 +4340,7 @@
       <c r="G357" s="12"/>
       <c r="H357" s="10"/>
     </row>
-    <row r="358" spans="1:8">
+    <row r="358" spans="1:8" ht="12.75">
       <c r="A358" s="11"/>
       <c r="B358" s="10"/>
       <c r="C358" s="11"/>
@@ -4347,7 +4350,7 @@
       <c r="G358" s="12"/>
       <c r="H358" s="10"/>
     </row>
-    <row r="359" spans="1:8">
+    <row r="359" spans="1:8" ht="12.75">
       <c r="A359" s="11"/>
       <c r="B359" s="10"/>
       <c r="C359" s="11"/>
@@ -4357,7 +4360,7 @@
       <c r="G359" s="12"/>
       <c r="H359" s="10"/>
     </row>
-    <row r="360" spans="1:8">
+    <row r="360" spans="1:8" ht="12.75">
       <c r="A360" s="11"/>
       <c r="B360" s="10"/>
       <c r="C360" s="11"/>
@@ -4367,7 +4370,7 @@
       <c r="G360" s="12"/>
       <c r="H360" s="10"/>
     </row>
-    <row r="361" spans="1:8">
+    <row r="361" spans="1:8" ht="12.75">
       <c r="A361" s="11"/>
       <c r="B361" s="10"/>
       <c r="C361" s="11"/>
@@ -4377,7 +4380,7 @@
       <c r="G361" s="12"/>
       <c r="H361" s="10"/>
     </row>
-    <row r="362" spans="1:8">
+    <row r="362" spans="1:8" ht="12.75">
       <c r="A362" s="11"/>
       <c r="B362" s="10"/>
       <c r="C362" s="11"/>
@@ -4387,7 +4390,7 @@
       <c r="G362" s="12"/>
       <c r="H362" s="10"/>
     </row>
-    <row r="363" spans="1:8">
+    <row r="363" spans="1:8" ht="12.75">
       <c r="A363" s="11"/>
       <c r="B363" s="10"/>
       <c r="C363" s="11"/>
@@ -4397,7 +4400,7 @@
       <c r="G363" s="12"/>
       <c r="H363" s="10"/>
     </row>
-    <row r="364" spans="1:8">
+    <row r="364" spans="1:8" ht="12.75">
       <c r="A364" s="11"/>
       <c r="B364" s="10"/>
       <c r="C364" s="11"/>
@@ -4407,7 +4410,7 @@
       <c r="G364" s="12"/>
       <c r="H364" s="10"/>
     </row>
-    <row r="365" spans="1:8">
+    <row r="365" spans="1:8" ht="12.75">
       <c r="A365" s="11"/>
       <c r="B365" s="10"/>
       <c r="C365" s="11"/>
@@ -4417,7 +4420,7 @@
       <c r="G365" s="12"/>
       <c r="H365" s="10"/>
     </row>
-    <row r="366" spans="1:8">
+    <row r="366" spans="1:8" ht="12.75">
       <c r="A366" s="11"/>
       <c r="B366" s="10"/>
       <c r="C366" s="11"/>
@@ -4427,7 +4430,7 @@
       <c r="G366" s="12"/>
       <c r="H366" s="10"/>
     </row>
-    <row r="367" spans="1:8">
+    <row r="367" spans="1:8" ht="12.75">
       <c r="A367" s="11"/>
       <c r="B367" s="10"/>
       <c r="C367" s="11"/>
@@ -4437,7 +4440,7 @@
       <c r="G367" s="12"/>
       <c r="H367" s="10"/>
     </row>
-    <row r="368" spans="1:8">
+    <row r="368" spans="1:8" ht="12.75">
       <c r="A368" s="11"/>
       <c r="B368" s="10"/>
       <c r="C368" s="11"/>
@@ -4447,7 +4450,7 @@
       <c r="G368" s="12"/>
       <c r="H368" s="10"/>
     </row>
-    <row r="369" spans="1:8">
+    <row r="369" spans="1:8" ht="12.75">
       <c r="A369" s="11"/>
       <c r="B369" s="10"/>
       <c r="C369" s="11"/>
@@ -4457,7 +4460,7 @@
       <c r="G369" s="12"/>
       <c r="H369" s="10"/>
     </row>
-    <row r="370" spans="1:8">
+    <row r="370" spans="1:8" ht="12.75">
       <c r="A370" s="11"/>
       <c r="B370" s="10"/>
       <c r="C370" s="11"/>
@@ -4467,7 +4470,7 @@
       <c r="G370" s="12"/>
       <c r="H370" s="10"/>
     </row>
-    <row r="371" spans="1:8">
+    <row r="371" spans="1:8" ht="12.75">
       <c r="A371" s="11"/>
       <c r="B371" s="10"/>
       <c r="C371" s="11"/>
@@ -4477,7 +4480,7 @@
       <c r="G371" s="12"/>
       <c r="H371" s="10"/>
     </row>
-    <row r="372" spans="1:8">
+    <row r="372" spans="1:8" ht="12.75">
       <c r="A372" s="11"/>
       <c r="B372" s="10"/>
       <c r="C372" s="11"/>
@@ -4487,7 +4490,7 @@
       <c r="G372" s="12"/>
       <c r="H372" s="10"/>
     </row>
-    <row r="373" spans="1:8">
+    <row r="373" spans="1:8" ht="12.75">
       <c r="A373" s="11"/>
       <c r="B373" s="10"/>
       <c r="C373" s="11"/>
@@ -4497,7 +4500,7 @@
       <c r="G373" s="12"/>
       <c r="H373" s="10"/>
     </row>
-    <row r="374" spans="1:8">
+    <row r="374" spans="1:8" ht="12.75">
       <c r="A374" s="11"/>
       <c r="B374" s="10"/>
       <c r="C374" s="11"/>
@@ -4507,7 +4510,7 @@
       <c r="G374" s="12"/>
       <c r="H374" s="10"/>
     </row>
-    <row r="375" spans="1:8">
+    <row r="375" spans="1:8" ht="12.75">
       <c r="A375" s="11"/>
       <c r="B375" s="10"/>
       <c r="C375" s="11"/>
@@ -4517,7 +4520,7 @@
       <c r="G375" s="12"/>
       <c r="H375" s="10"/>
     </row>
-    <row r="376" spans="1:8">
+    <row r="376" spans="1:8" ht="12.75">
       <c r="A376" s="11"/>
       <c r="B376" s="10"/>
       <c r="C376" s="11"/>
@@ -4527,7 +4530,7 @@
       <c r="G376" s="12"/>
       <c r="H376" s="10"/>
     </row>
-    <row r="377" spans="1:8">
+    <row r="377" spans="1:8" ht="12.75">
       <c r="A377" s="11"/>
       <c r="B377" s="10"/>
       <c r="C377" s="11"/>
@@ -4537,7 +4540,7 @@
       <c r="G377" s="12"/>
       <c r="H377" s="10"/>
     </row>
-    <row r="378" spans="1:8">
+    <row r="378" spans="1:8" ht="12.75">
       <c r="A378" s="11"/>
       <c r="B378" s="10"/>
       <c r="C378" s="11"/>
@@ -4547,7 +4550,7 @@
       <c r="G378" s="12"/>
       <c r="H378" s="10"/>
     </row>
-    <row r="379" spans="1:8">
+    <row r="379" spans="1:8" ht="12.75">
       <c r="A379" s="11"/>
       <c r="B379" s="10"/>
       <c r="C379" s="11"/>
@@ -4557,7 +4560,7 @@
       <c r="G379" s="12"/>
       <c r="H379" s="10"/>
     </row>
-    <row r="380" spans="1:8">
+    <row r="380" spans="1:8" ht="12.75">
       <c r="A380" s="11"/>
       <c r="B380" s="10"/>
       <c r="C380" s="11"/>
@@ -4567,7 +4570,7 @@
       <c r="G380" s="12"/>
       <c r="H380" s="10"/>
     </row>
-    <row r="381" spans="1:8">
+    <row r="381" spans="1:8" ht="12.75">
       <c r="A381" s="11"/>
       <c r="B381" s="10"/>
       <c r="C381" s="11"/>
@@ -4577,7 +4580,7 @@
       <c r="G381" s="12"/>
       <c r="H381" s="10"/>
     </row>
-    <row r="382" spans="1:8">
+    <row r="382" spans="1:8" ht="12.75">
       <c r="A382" s="11"/>
       <c r="B382" s="10"/>
       <c r="C382" s="11"/>
@@ -4587,7 +4590,7 @@
       <c r="G382" s="12"/>
       <c r="H382" s="10"/>
     </row>
-    <row r="383" spans="1:8">
+    <row r="383" spans="1:8" ht="12.75">
       <c r="A383" s="11"/>
       <c r="B383" s="10"/>
       <c r="C383" s="11"/>
@@ -4597,7 +4600,7 @@
       <c r="G383" s="12"/>
       <c r="H383" s="10"/>
     </row>
-    <row r="384" spans="1:8">
+    <row r="384" spans="1:8" ht="12.75">
       <c r="A384" s="11"/>
       <c r="B384" s="10"/>
       <c r="C384" s="11"/>
@@ -4607,7 +4610,7 @@
       <c r="G384" s="12"/>
       <c r="H384" s="10"/>
     </row>
-    <row r="385" spans="1:8">
+    <row r="385" spans="1:8" ht="12.75">
       <c r="A385" s="11"/>
       <c r="B385" s="10"/>
       <c r="C385" s="11"/>
@@ -4617,7 +4620,7 @@
       <c r="G385" s="12"/>
       <c r="H385" s="10"/>
     </row>
-    <row r="386" spans="1:8">
+    <row r="386" spans="1:8" ht="12.75">
       <c r="A386" s="11"/>
       <c r="B386" s="10"/>
       <c r="C386" s="11"/>
@@ -4627,7 +4630,7 @@
       <c r="G386" s="12"/>
       <c r="H386" s="10"/>
     </row>
-    <row r="387" spans="1:8">
+    <row r="387" spans="1:8" ht="12.75">
       <c r="A387" s="11"/>
       <c r="B387" s="10"/>
       <c r="C387" s="11"/>
@@ -4637,7 +4640,7 @@
       <c r="G387" s="12"/>
       <c r="H387" s="10"/>
     </row>
-    <row r="388" spans="1:8">
+    <row r="388" spans="1:8" ht="12.75">
       <c r="A388" s="11"/>
       <c r="B388" s="10"/>
       <c r="C388" s="11"/>
@@ -4647,7 +4650,7 @@
       <c r="G388" s="12"/>
       <c r="H388" s="10"/>
     </row>
-    <row r="389" spans="1:8">
+    <row r="389" spans="1:8" ht="12.75">
       <c r="A389" s="11"/>
       <c r="B389" s="10"/>
       <c r="C389" s="11"/>
@@ -4657,7 +4660,7 @@
       <c r="G389" s="12"/>
       <c r="H389" s="10"/>
     </row>
-    <row r="390" spans="1:8">
+    <row r="390" spans="1:8" ht="12.75">
       <c r="A390" s="11"/>
       <c r="B390" s="10"/>
       <c r="C390" s="11"/>
@@ -4667,7 +4670,7 @@
       <c r="G390" s="12"/>
       <c r="H390" s="10"/>
     </row>
-    <row r="391" spans="1:8">
+    <row r="391" spans="1:8" ht="12.75">
       <c r="A391" s="11"/>
       <c r="B391" s="10"/>
       <c r="C391" s="11"/>
@@ -4677,7 +4680,7 @@
       <c r="G391" s="12"/>
       <c r="H391" s="10"/>
     </row>
-    <row r="392" spans="1:8">
+    <row r="392" spans="1:8" ht="12.75">
       <c r="A392" s="11"/>
       <c r="B392" s="10"/>
       <c r="C392" s="11"/>
@@ -4687,7 +4690,7 @@
       <c r="G392" s="12"/>
       <c r="H392" s="10"/>
     </row>
-    <row r="393" spans="1:8">
+    <row r="393" spans="1:8" ht="12.75">
       <c r="A393" s="11"/>
       <c r="B393" s="10"/>
       <c r="C393" s="11"/>
@@ -4697,7 +4700,7 @@
       <c r="G393" s="12"/>
       <c r="H393" s="10"/>
     </row>
-    <row r="394" spans="1:8">
+    <row r="394" spans="1:8" ht="12.75">
       <c r="A394" s="11"/>
       <c r="B394" s="10"/>
       <c r="C394" s="11"/>
@@ -4707,7 +4710,7 @@
       <c r="G394" s="12"/>
       <c r="H394" s="10"/>
     </row>
-    <row r="395" spans="1:8">
+    <row r="395" spans="1:8" ht="12.75">
       <c r="A395" s="11"/>
       <c r="B395" s="10"/>
       <c r="C395" s="11"/>
@@ -4717,7 +4720,7 @@
       <c r="G395" s="12"/>
       <c r="H395" s="10"/>
     </row>
-    <row r="396" spans="1:8">
+    <row r="396" spans="1:8" ht="12.75">
       <c r="A396" s="11"/>
       <c r="B396" s="10"/>
       <c r="C396" s="11"/>
@@ -4727,7 +4730,7 @@
       <c r="G396" s="12"/>
       <c r="H396" s="10"/>
     </row>
-    <row r="397" spans="1:8">
+    <row r="397" spans="1:8" ht="12.75">
       <c r="A397" s="11"/>
       <c r="B397" s="10"/>
       <c r="C397" s="11"/>
@@ -4737,7 +4740,7 @@
       <c r="G397" s="12"/>
       <c r="H397" s="10"/>
     </row>
-    <row r="398" spans="1:8">
+    <row r="398" spans="1:8" ht="12.75">
       <c r="A398" s="11"/>
       <c r="B398" s="10"/>
       <c r="C398" s="11"/>
@@ -4747,7 +4750,7 @@
       <c r="G398" s="12"/>
       <c r="H398" s="10"/>
     </row>
-    <row r="399" spans="1:8">
+    <row r="399" spans="1:8" ht="12.75">
       <c r="A399" s="11"/>
       <c r="B399" s="10"/>
       <c r="C399" s="11"/>
@@ -4757,7 +4760,7 @@
       <c r="G399" s="12"/>
       <c r="H399" s="10"/>
     </row>
-    <row r="400" spans="1:8">
+    <row r="400" spans="1:8" ht="12.75">
       <c r="A400" s="11"/>
       <c r="B400" s="10"/>
       <c r="C400" s="11"/>
@@ -4767,7 +4770,7 @@
       <c r="G400" s="12"/>
       <c r="H400" s="10"/>
     </row>
-    <row r="401" spans="1:8">
+    <row r="401" spans="1:8" ht="12.75">
       <c r="A401" s="11"/>
       <c r="B401" s="10"/>
       <c r="C401" s="11"/>
@@ -4777,7 +4780,7 @@
       <c r="G401" s="12"/>
       <c r="H401" s="10"/>
     </row>
-    <row r="402" spans="1:8">
+    <row r="402" spans="1:8" ht="12.75">
       <c r="A402" s="11"/>
       <c r="B402" s="10"/>
       <c r="C402" s="11"/>
@@ -4787,7 +4790,7 @@
       <c r="G402" s="12"/>
       <c r="H402" s="10"/>
     </row>
-    <row r="403" spans="1:8">
+    <row r="403" spans="1:8" ht="12.75">
       <c r="A403" s="11"/>
       <c r="B403" s="10"/>
       <c r="C403" s="11"/>
@@ -4797,7 +4800,7 @@
       <c r="G403" s="12"/>
       <c r="H403" s="10"/>
     </row>
-    <row r="404" spans="1:8">
+    <row r="404" spans="1:8" ht="12.75">
       <c r="A404" s="11"/>
       <c r="B404" s="10"/>
       <c r="C404" s="11"/>
@@ -4807,7 +4810,7 @@
       <c r="G404" s="12"/>
       <c r="H404" s="10"/>
     </row>
-    <row r="405" spans="1:8">
+    <row r="405" spans="1:8" ht="12.75">
       <c r="A405" s="11"/>
       <c r="B405" s="10"/>
       <c r="C405" s="11"/>
@@ -4817,7 +4820,7 @@
       <c r="G405" s="12"/>
       <c r="H405" s="10"/>
     </row>
-    <row r="406" spans="1:8">
+    <row r="406" spans="1:8" ht="12.75">
       <c r="A406" s="11"/>
       <c r="B406" s="10"/>
       <c r="C406" s="11"/>
@@ -4827,7 +4830,7 @@
       <c r="G406" s="12"/>
       <c r="H406" s="10"/>
     </row>
-    <row r="407" spans="1:8">
+    <row r="407" spans="1:8" ht="12.75">
       <c r="A407" s="11"/>
       <c r="B407" s="10"/>
       <c r="C407" s="11"/>
@@ -4837,7 +4840,7 @@
       <c r="G407" s="12"/>
       <c r="H407" s="10"/>
     </row>
-    <row r="408" spans="1:8">
+    <row r="408" spans="1:8" ht="12.75">
       <c r="A408" s="11"/>
       <c r="B408" s="10"/>
       <c r="C408" s="11"/>
@@ -4847,7 +4850,7 @@
       <c r="G408" s="12"/>
       <c r="H408" s="10"/>
     </row>
-    <row r="409" spans="1:8">
+    <row r="409" spans="1:8" ht="12.75">
       <c r="A409" s="11"/>
       <c r="B409" s="10"/>
       <c r="C409" s="11"/>
@@ -4857,7 +4860,7 @@
       <c r="G409" s="12"/>
       <c r="H409" s="10"/>
     </row>
-    <row r="410" spans="1:8">
+    <row r="410" spans="1:8" ht="12.75">
       <c r="A410" s="11"/>
       <c r="B410" s="10"/>
       <c r="C410" s="11"/>
@@ -4867,7 +4870,7 @@
       <c r="G410" s="12"/>
       <c r="H410" s="10"/>
     </row>
-    <row r="411" spans="1:8">
+    <row r="411" spans="1:8" ht="12.75">
       <c r="A411" s="11"/>
       <c r="B411" s="10"/>
       <c r="C411" s="11"/>
@@ -4877,7 +4880,7 @@
       <c r="G411" s="12"/>
       <c r="H411" s="10"/>
     </row>
-    <row r="412" spans="1:8">
+    <row r="412" spans="1:8" ht="12.75">
       <c r="A412" s="11"/>
       <c r="B412" s="10"/>
       <c r="C412" s="11"/>
@@ -4887,7 +4890,7 @@
       <c r="G412" s="12"/>
       <c r="H412" s="10"/>
     </row>
-    <row r="413" spans="1:8">
+    <row r="413" spans="1:8" ht="12.75">
       <c r="A413" s="11"/>
       <c r="B413" s="10"/>
       <c r="C413" s="11"/>
@@ -4897,7 +4900,7 @@
       <c r="G413" s="12"/>
       <c r="H413" s="10"/>
     </row>
-    <row r="414" spans="1:8">
+    <row r="414" spans="1:8" ht="12.75">
       <c r="A414" s="11"/>
       <c r="B414" s="10"/>
       <c r="C414" s="11"/>
@@ -4907,7 +4910,7 @@
       <c r="G414" s="12"/>
       <c r="H414" s="10"/>
     </row>
-    <row r="415" spans="1:8">
+    <row r="415" spans="1:8" ht="12.75">
       <c r="A415" s="11"/>
       <c r="B415" s="10"/>
       <c r="C415" s="11"/>
@@ -4917,7 +4920,7 @@
       <c r="G415" s="12"/>
       <c r="H415" s="10"/>
     </row>
-    <row r="416" spans="1:8">
+    <row r="416" spans="1:8" ht="12.75">
       <c r="A416" s="11"/>
       <c r="B416" s="10"/>
       <c r="C416" s="11"/>
@@ -4927,7 +4930,7 @@
       <c r="G416" s="12"/>
       <c r="H416" s="10"/>
     </row>
-    <row r="417" spans="1:8">
+    <row r="417" spans="1:8" ht="12.75">
       <c r="A417" s="11"/>
       <c r="B417" s="10"/>
       <c r="C417" s="11"/>
@@ -4937,7 +4940,7 @@
       <c r="G417" s="12"/>
       <c r="H417" s="10"/>
     </row>
-    <row r="418" spans="1:8">
+    <row r="418" spans="1:8" ht="12.75">
       <c r="A418" s="11"/>
       <c r="B418" s="10"/>
       <c r="C418" s="11"/>
@@ -4947,7 +4950,7 @@
       <c r="G418" s="12"/>
       <c r="H418" s="10"/>
     </row>
-    <row r="419" spans="1:8">
+    <row r="419" spans="1:8" ht="12.75">
       <c r="A419" s="11"/>
       <c r="B419" s="10"/>
       <c r="C419" s="11"/>
@@ -4957,7 +4960,7 @@
       <c r="G419" s="12"/>
       <c r="H419" s="10"/>
     </row>
-    <row r="420" spans="1:8">
+    <row r="420" spans="1:8" ht="12.75">
       <c r="A420" s="11"/>
       <c r="B420" s="10"/>
       <c r="C420" s="11"/>
@@ -4967,7 +4970,7 @@
       <c r="G420" s="12"/>
       <c r="H420" s="10"/>
     </row>
-    <row r="421" spans="1:8">
+    <row r="421" spans="1:8" ht="12.75">
       <c r="A421" s="11"/>
       <c r="B421" s="10"/>
       <c r="C421" s="11"/>
@@ -4977,7 +4980,7 @@
       <c r="G421" s="12"/>
       <c r="H421" s="10"/>
     </row>
-    <row r="422" spans="1:8">
+    <row r="422" spans="1:8" ht="12.75">
       <c r="A422" s="11"/>
       <c r="B422" s="10"/>
       <c r="C422" s="11"/>
@@ -4987,7 +4990,7 @@
       <c r="G422" s="12"/>
       <c r="H422" s="10"/>
     </row>
-    <row r="423" spans="1:8">
+    <row r="423" spans="1:8" ht="12.75">
       <c r="A423" s="11"/>
       <c r="B423" s="10"/>
       <c r="C423" s="11"/>
@@ -4997,7 +5000,7 @@
       <c r="G423" s="12"/>
       <c r="H423" s="10"/>
     </row>
-    <row r="424" spans="1:8">
+    <row r="424" spans="1:8" ht="12.75">
       <c r="A424" s="11"/>
       <c r="B424" s="10"/>
       <c r="C424" s="11"/>
@@ -5007,7 +5010,7 @@
       <c r="G424" s="12"/>
       <c r="H424" s="10"/>
     </row>
-    <row r="425" spans="1:8">
+    <row r="425" spans="1:8" ht="12.75">
       <c r="A425" s="11"/>
       <c r="B425" s="10"/>
       <c r="C425" s="11"/>
@@ -5017,7 +5020,7 @@
       <c r="G425" s="12"/>
       <c r="H425" s="10"/>
     </row>
-    <row r="426" spans="1:8">
+    <row r="426" spans="1:8" ht="12.75">
       <c r="A426" s="11"/>
       <c r="B426" s="10"/>
       <c r="C426" s="11"/>
@@ -5027,7 +5030,7 @@
       <c r="G426" s="12"/>
       <c r="H426" s="10"/>
     </row>
-    <row r="427" spans="1:8">
+    <row r="427" spans="1:8" ht="12.75">
       <c r="A427" s="11"/>
       <c r="B427" s="10"/>
       <c r="C427" s="11"/>
@@ -5037,7 +5040,7 @@
       <c r="G427" s="12"/>
       <c r="H427" s="10"/>
     </row>
-    <row r="428" spans="1:8">
+    <row r="428" spans="1:8" ht="12.75">
       <c r="A428" s="11"/>
       <c r="B428" s="10"/>
       <c r="C428" s="11"/>
@@ -5047,7 +5050,7 @@
       <c r="G428" s="12"/>
       <c r="H428" s="10"/>
     </row>
-    <row r="429" spans="1:8">
+    <row r="429" spans="1:8" ht="12.75">
       <c r="A429" s="11"/>
       <c r="B429" s="10"/>
       <c r="C429" s="11"/>
@@ -5057,7 +5060,7 @@
       <c r="G429" s="12"/>
       <c r="H429" s="10"/>
     </row>
-    <row r="430" spans="1:8">
+    <row r="430" spans="1:8" ht="12.75">
       <c r="A430" s="11"/>
       <c r="B430" s="10"/>
       <c r="C430" s="11"/>
@@ -5067,7 +5070,7 @@
       <c r="G430" s="12"/>
       <c r="H430" s="10"/>
     </row>
-    <row r="431" spans="1:8">
+    <row r="431" spans="1:8" ht="12.75">
       <c r="A431" s="11"/>
       <c r="B431" s="10"/>
       <c r="C431" s="11"/>
@@ -5077,7 +5080,7 @@
       <c r="G431" s="12"/>
       <c r="H431" s="10"/>
     </row>
-    <row r="432" spans="1:8">
+    <row r="432" spans="1:8" ht="12.75">
       <c r="A432" s="11"/>
       <c r="B432" s="10"/>
       <c r="C432" s="11"/>
@@ -5087,7 +5090,7 @@
       <c r="G432" s="12"/>
       <c r="H432" s="10"/>
     </row>
-    <row r="433" spans="1:8">
+    <row r="433" spans="1:8" ht="12.75">
       <c r="A433" s="11"/>
       <c r="B433" s="10"/>
       <c r="C433" s="11"/>
@@ -5097,7 +5100,7 @@
       <c r="G433" s="12"/>
       <c r="H433" s="10"/>
     </row>
-    <row r="434" spans="1:8">
+    <row r="434" spans="1:8" ht="12.75">
       <c r="A434" s="11"/>
       <c r="B434" s="10"/>
       <c r="C434" s="11"/>
@@ -5107,7 +5110,7 @@
       <c r="G434" s="12"/>
       <c r="H434" s="10"/>
     </row>
-    <row r="435" spans="1:8">
+    <row r="435" spans="1:8" ht="12.75">
       <c r="A435" s="11"/>
       <c r="B435" s="10"/>
       <c r="C435" s="11"/>
@@ -5117,7 +5120,7 @@
       <c r="G435" s="12"/>
       <c r="H435" s="10"/>
     </row>
-    <row r="436" spans="1:8">
+    <row r="436" spans="1:8" ht="12.75">
       <c r="A436" s="11"/>
       <c r="B436" s="10"/>
       <c r="C436" s="11"/>
@@ -5127,7 +5130,7 @@
       <c r="G436" s="12"/>
       <c r="H436" s="10"/>
     </row>
-    <row r="437" spans="1:8">
+    <row r="437" spans="1:8" ht="12.75">
       <c r="A437" s="11"/>
       <c r="B437" s="10"/>
       <c r="C437" s="11"/>
@@ -5137,7 +5140,7 @@
       <c r="G437" s="12"/>
       <c r="H437" s="10"/>
     </row>
-    <row r="438" spans="1:8">
+    <row r="438" spans="1:8" ht="12.75">
       <c r="A438" s="11"/>
       <c r="B438" s="10"/>
       <c r="C438" s="11"/>
@@ -5147,7 +5150,7 @@
       <c r="G438" s="12"/>
       <c r="H438" s="10"/>
     </row>
-    <row r="439" spans="1:8">
+    <row r="439" spans="1:8" ht="12.75">
       <c r="A439" s="11"/>
       <c r="B439" s="10"/>
       <c r="C439" s="11"/>
@@ -5157,7 +5160,7 @@
       <c r="G439" s="12"/>
       <c r="H439" s="10"/>
     </row>
-    <row r="440" spans="1:8">
+    <row r="440" spans="1:8" ht="12.75">
       <c r="A440" s="11"/>
       <c r="B440" s="10"/>
       <c r="C440" s="11"/>
@@ -5167,7 +5170,7 @@
       <c r="G440" s="12"/>
       <c r="H440" s="10"/>
     </row>
-    <row r="441" spans="1:8">
+    <row r="441" spans="1:8" ht="12.75">
       <c r="A441" s="11"/>
       <c r="B441" s="10"/>
       <c r="C441" s="11"/>
@@ -5177,7 +5180,7 @@
       <c r="G441" s="12"/>
       <c r="H441" s="10"/>
     </row>
-    <row r="442" spans="1:8">
+    <row r="442" spans="1:8" ht="12.75">
       <c r="A442" s="11"/>
       <c r="B442" s="10"/>
       <c r="C442" s="11"/>
@@ -5187,7 +5190,7 @@
       <c r="G442" s="12"/>
       <c r="H442" s="10"/>
     </row>
-    <row r="443" spans="1:8">
+    <row r="443" spans="1:8" ht="12.75">
       <c r="A443" s="11"/>
       <c r="B443" s="10"/>
       <c r="C443" s="11"/>
@@ -5197,7 +5200,7 @@
       <c r="G443" s="12"/>
       <c r="H443" s="10"/>
     </row>
-    <row r="444" spans="1:8">
+    <row r="444" spans="1:8" ht="12.75">
       <c r="A444" s="11"/>
       <c r="B444" s="10"/>
       <c r="C444" s="11"/>
@@ -5207,7 +5210,7 @@
       <c r="G444" s="12"/>
       <c r="H444" s="10"/>
     </row>
-    <row r="445" spans="1:8">
+    <row r="445" spans="1:8" ht="12.75">
       <c r="A445" s="11"/>
       <c r="B445" s="10"/>
       <c r="C445" s="11"/>
@@ -5217,7 +5220,7 @@
       <c r="G445" s="12"/>
       <c r="H445" s="10"/>
     </row>
-    <row r="446" spans="1:8">
+    <row r="446" spans="1:8" ht="12.75">
       <c r="A446" s="11"/>
       <c r="B446" s="10"/>
       <c r="C446" s="11"/>
@@ -5227,7 +5230,7 @@
       <c r="G446" s="12"/>
       <c r="H446" s="10"/>
     </row>
-    <row r="447" spans="1:8">
+    <row r="447" spans="1:8" ht="12.75">
       <c r="A447" s="11"/>
       <c r="B447" s="10"/>
       <c r="C447" s="11"/>
@@ -5237,7 +5240,7 @@
       <c r="G447" s="12"/>
       <c r="H447" s="10"/>
     </row>
-    <row r="448" spans="1:8">
+    <row r="448" spans="1:8" ht="12.75">
       <c r="A448" s="11"/>
       <c r="B448" s="10"/>
       <c r="C448" s="11"/>
@@ -5247,7 +5250,7 @@
       <c r="G448" s="12"/>
       <c r="H448" s="10"/>
     </row>
-    <row r="449" spans="1:8">
+    <row r="449" spans="1:8" ht="12.75">
       <c r="A449" s="11"/>
       <c r="B449" s="10"/>
       <c r="C449" s="11"/>
@@ -5257,7 +5260,7 @@
       <c r="G449" s="12"/>
       <c r="H449" s="10"/>
     </row>
-    <row r="450" spans="1:8">
+    <row r="450" spans="1:8" ht="12.75">
       <c r="A450" s="11"/>
       <c r="B450" s="10"/>
       <c r="C450" s="11"/>
@@ -5267,7 +5270,7 @@
       <c r="G450" s="12"/>
       <c r="H450" s="10"/>
     </row>
-    <row r="451" spans="1:8">
+    <row r="451" spans="1:8" ht="12.75">
       <c r="A451" s="11"/>
       <c r="B451" s="10"/>
       <c r="C451" s="11"/>
@@ -5277,7 +5280,7 @@
       <c r="G451" s="12"/>
       <c r="H451" s="10"/>
     </row>
-    <row r="452" spans="1:8">
+    <row r="452" spans="1:8" ht="12.75">
       <c r="A452" s="11"/>
       <c r="B452" s="10"/>
       <c r="C452" s="11"/>
@@ -5287,7 +5290,7 @@
       <c r="G452" s="12"/>
       <c r="H452" s="10"/>
     </row>
-    <row r="453" spans="1:8">
+    <row r="453" spans="1:8" ht="12.75">
       <c r="A453" s="11"/>
       <c r="B453" s="10"/>
       <c r="C453" s="11"/>
@@ -5297,7 +5300,7 @@
       <c r="G453" s="12"/>
       <c r="H453" s="10"/>
     </row>
-    <row r="454" spans="1:8">
+    <row r="454" spans="1:8" ht="12.75">
       <c r="A454" s="11"/>
       <c r="B454" s="10"/>
       <c r="C454" s="11"/>
@@ -5307,7 +5310,7 @@
       <c r="G454" s="12"/>
       <c r="H454" s="10"/>
     </row>
-    <row r="455" spans="1:8">
+    <row r="455" spans="1:8" ht="12.75">
       <c r="A455" s="11"/>
       <c r="B455" s="10"/>
       <c r="C455" s="11"/>
@@ -5317,7 +5320,7 @@
       <c r="G455" s="12"/>
       <c r="H455" s="10"/>
     </row>
-    <row r="456" spans="1:8">
+    <row r="456" spans="1:8" ht="12.75">
       <c r="A456" s="11"/>
       <c r="B456" s="10"/>
       <c r="C456" s="11"/>
@@ -5327,7 +5330,7 @@
       <c r="G456" s="12"/>
       <c r="H456" s="10"/>
     </row>
-    <row r="457" spans="1:8">
+    <row r="457" spans="1:8" ht="12.75">
       <c r="A457" s="11"/>
       <c r="B457" s="10"/>
       <c r="C457" s="11"/>
@@ -5337,7 +5340,7 @@
       <c r="G457" s="12"/>
       <c r="H457" s="10"/>
     </row>
-    <row r="458" spans="1:8">
+    <row r="458" spans="1:8" ht="12.75">
       <c r="A458" s="11"/>
       <c r="B458" s="10"/>
       <c r="C458" s="11"/>
@@ -5347,7 +5350,7 @@
       <c r="G458" s="12"/>
       <c r="H458" s="10"/>
     </row>
-    <row r="459" spans="1:8">
+    <row r="459" spans="1:8" ht="12.75">
       <c r="A459" s="11"/>
       <c r="B459" s="10"/>
       <c r="C459" s="11"/>
@@ -5357,7 +5360,7 @@
       <c r="G459" s="12"/>
       <c r="H459" s="10"/>
     </row>
-    <row r="460" spans="1:8">
+    <row r="460" spans="1:8" ht="12.75">
       <c r="A460" s="11"/>
       <c r="B460" s="10"/>
       <c r="C460" s="11"/>
@@ -5367,7 +5370,7 @@
       <c r="G460" s="12"/>
       <c r="H460" s="10"/>
     </row>
-    <row r="461" spans="1:8">
+    <row r="461" spans="1:8" ht="12.75">
       <c r="A461" s="11"/>
       <c r="B461" s="10"/>
       <c r="C461" s="11"/>
@@ -5377,7 +5380,7 @@
       <c r="G461" s="12"/>
       <c r="H461" s="10"/>
     </row>
-    <row r="462" spans="1:8">
+    <row r="462" spans="1:8" ht="12.75">
       <c r="A462" s="11"/>
       <c r="B462" s="10"/>
       <c r="C462" s="11"/>
@@ -5387,7 +5390,7 @@
       <c r="G462" s="12"/>
       <c r="H462" s="10"/>
     </row>
-    <row r="463" spans="1:8">
+    <row r="463" spans="1:8" ht="12.75">
       <c r="A463" s="11"/>
       <c r="B463" s="10"/>
       <c r="C463" s="11"/>
@@ -5397,7 +5400,7 @@
       <c r="G463" s="12"/>
       <c r="H463" s="10"/>
     </row>
-    <row r="464" spans="1:8">
+    <row r="464" spans="1:8" ht="12.75">
       <c r="A464" s="11"/>
       <c r="B464" s="10"/>
       <c r="C464" s="11"/>
@@ -5407,7 +5410,7 @@
       <c r="G464" s="12"/>
       <c r="H464" s="10"/>
     </row>
-    <row r="465" spans="1:8">
+    <row r="465" spans="1:8" ht="12.75">
       <c r="A465" s="11"/>
       <c r="B465" s="10"/>
       <c r="C465" s="11"/>
@@ -5417,7 +5420,7 @@
       <c r="G465" s="12"/>
       <c r="H465" s="10"/>
     </row>
-    <row r="466" spans="1:8">
+    <row r="466" spans="1:8" ht="12.75">
       <c r="A466" s="11"/>
       <c r="B466" s="10"/>
       <c r="C466" s="11"/>
@@ -5427,7 +5430,7 @@
       <c r="G466" s="12"/>
       <c r="H466" s="10"/>
     </row>
-    <row r="467" spans="1:8">
+    <row r="467" spans="1:8" ht="12.75">
       <c r="A467" s="11"/>
       <c r="B467" s="10"/>
       <c r="C467" s="11"/>
@@ -5437,7 +5440,7 @@
       <c r="G467" s="12"/>
       <c r="H467" s="10"/>
     </row>
-    <row r="468" spans="1:8">
+    <row r="468" spans="1:8" ht="12.75">
       <c r="A468" s="11"/>
       <c r="B468" s="10"/>
       <c r="C468" s="11"/>
@@ -5447,7 +5450,7 @@
       <c r="G468" s="12"/>
       <c r="H468" s="10"/>
     </row>
-    <row r="469" spans="1:8">
+    <row r="469" spans="1:8" ht="12.75">
       <c r="A469" s="11"/>
       <c r="B469" s="10"/>
       <c r="C469" s="11"/>
@@ -5457,7 +5460,7 @@
       <c r="G469" s="12"/>
       <c r="H469" s="10"/>
     </row>
-    <row r="470" spans="1:8">
+    <row r="470" spans="1:8" ht="12.75">
       <c r="A470" s="11"/>
       <c r="B470" s="10"/>
       <c r="C470" s="11"/>
@@ -5467,7 +5470,7 @@
       <c r="G470" s="12"/>
       <c r="H470" s="10"/>
     </row>
-    <row r="471" spans="1:8">
+    <row r="471" spans="1:8" ht="12.75">
       <c r="A471" s="11"/>
       <c r="B471" s="10"/>
       <c r="C471" s="11"/>
@@ -5477,7 +5480,7 @@
       <c r="G471" s="12"/>
       <c r="H471" s="10"/>
     </row>
-    <row r="472" spans="1:8">
+    <row r="472" spans="1:8" ht="12.75">
       <c r="A472" s="11"/>
       <c r="B472" s="10"/>
       <c r="C472" s="11"/>
@@ -5487,7 +5490,7 @@
       <c r="G472" s="12"/>
       <c r="H472" s="10"/>
     </row>
-    <row r="473" spans="1:8">
+    <row r="473" spans="1:8" ht="12.75">
       <c r="A473" s="11"/>
       <c r="B473" s="10"/>
       <c r="C473" s="11"/>
@@ -5497,7 +5500,7 @@
       <c r="G473" s="12"/>
       <c r="H473" s="10"/>
     </row>
-    <row r="474" spans="1:8">
+    <row r="474" spans="1:8" ht="12.75">
       <c r="A474" s="11"/>
       <c r="B474" s="10"/>
       <c r="C474" s="11"/>
@@ -5507,7 +5510,7 @@
       <c r="G474" s="12"/>
       <c r="H474" s="10"/>
     </row>
-    <row r="475" spans="1:8">
+    <row r="475" spans="1:8" ht="12.75">
       <c r="A475" s="11"/>
       <c r="B475" s="10"/>
       <c r="C475" s="11"/>
@@ -5517,7 +5520,7 @@
       <c r="G475" s="12"/>
       <c r="H475" s="10"/>
     </row>
-    <row r="476" spans="1:8">
+    <row r="476" spans="1:8" ht="12.75">
       <c r="A476" s="11"/>
       <c r="B476" s="10"/>
       <c r="C476" s="11"/>
@@ -5527,7 +5530,7 @@
       <c r="G476" s="12"/>
       <c r="H476" s="10"/>
     </row>
-    <row r="477" spans="1:8">
+    <row r="477" spans="1:8" ht="12.75">
       <c r="A477" s="11"/>
       <c r="B477" s="10"/>
       <c r="C477" s="11"/>
@@ -5537,7 +5540,7 @@
       <c r="G477" s="12"/>
       <c r="H477" s="10"/>
     </row>
-    <row r="478" spans="1:8">
+    <row r="478" spans="1:8" ht="12.75">
       <c r="A478" s="11"/>
       <c r="B478" s="10"/>
       <c r="C478" s="11"/>
@@ -5547,7 +5550,7 @@
       <c r="G478" s="12"/>
       <c r="H478" s="10"/>
     </row>
-    <row r="479" spans="1:8">
+    <row r="479" spans="1:8" ht="12.75">
       <c r="A479" s="11"/>
       <c r="B479" s="10"/>
       <c r="C479" s="11"/>
@@ -5557,7 +5560,7 @@
       <c r="G479" s="12"/>
       <c r="H479" s="10"/>
     </row>
-    <row r="480" spans="1:8">
+    <row r="480" spans="1:8" ht="12.75">
       <c r="A480" s="11"/>
       <c r="B480" s="10"/>
       <c r="C480" s="11"/>
@@ -5567,7 +5570,7 @@
       <c r="G480" s="12"/>
       <c r="H480" s="10"/>
     </row>
-    <row r="481" spans="1:8">
+    <row r="481" spans="1:8" ht="12.75">
       <c r="A481" s="11"/>
       <c r="B481" s="10"/>
       <c r="C481" s="11"/>
@@ -5577,7 +5580,7 @@
       <c r="G481" s="12"/>
       <c r="H481" s="10"/>
     </row>
-    <row r="482" spans="1:8">
+    <row r="482" spans="1:8" ht="12.75">
       <c r="A482" s="11"/>
       <c r="B482" s="10"/>
       <c r="C482" s="11"/>
@@ -5587,7 +5590,7 @@
       <c r="G482" s="12"/>
       <c r="H482" s="10"/>
     </row>
-    <row r="483" spans="1:8">
+    <row r="483" spans="1:8" ht="12.75">
       <c r="A483" s="11"/>
       <c r="B483" s="10"/>
       <c r="C483" s="11"/>
@@ -5597,7 +5600,7 @@
       <c r="G483" s="12"/>
       <c r="H483" s="10"/>
     </row>
-    <row r="484" spans="1:8">
+    <row r="484" spans="1:8" ht="12.75">
       <c r="A484" s="11"/>
       <c r="B484" s="10"/>
       <c r="C484" s="11"/>
@@ -5607,7 +5610,7 @@
       <c r="G484" s="12"/>
       <c r="H484" s="10"/>
     </row>
-    <row r="485" spans="1:8">
+    <row r="485" spans="1:8" ht="12.75">
       <c r="A485" s="11"/>
       <c r="B485" s="10"/>
       <c r="C485" s="11"/>
@@ -5617,7 +5620,7 @@
       <c r="G485" s="12"/>
       <c r="H485" s="10"/>
     </row>
-    <row r="486" spans="1:8">
+    <row r="486" spans="1:8" ht="12.75">
       <c r="A486" s="11"/>
       <c r="B486" s="10"/>
       <c r="C486" s="11"/>
@@ -5627,7 +5630,7 @@
       <c r="G486" s="12"/>
       <c r="H486" s="10"/>
     </row>
-    <row r="487" spans="1:8">
+    <row r="487" spans="1:8" ht="12.75">
       <c r="A487" s="11"/>
       <c r="B487" s="10"/>
       <c r="C487" s="11"/>
@@ -5637,7 +5640,7 @@
       <c r="G487" s="12"/>
       <c r="H487" s="10"/>
     </row>
-    <row r="488" spans="1:8">
+    <row r="488" spans="1:8" ht="12.75">
       <c r="A488" s="11"/>
       <c r="B488" s="10"/>
       <c r="C488" s="11"/>
@@ -5647,7 +5650,7 @@
       <c r="G488" s="12"/>
       <c r="H488" s="10"/>
     </row>
-    <row r="489" spans="1:8">
+    <row r="489" spans="1:8" ht="12.75">
       <c r="A489" s="11"/>
       <c r="B489" s="10"/>
       <c r="C489" s="11"/>
@@ -5657,7 +5660,7 @@
       <c r="G489" s="12"/>
       <c r="H489" s="10"/>
     </row>
-    <row r="490" spans="1:8">
+    <row r="490" spans="1:8" ht="12.75">
       <c r="A490" s="11"/>
       <c r="B490" s="10"/>
       <c r="C490" s="11"/>
@@ -5667,7 +5670,7 @@
       <c r="G490" s="12"/>
       <c r="H490" s="10"/>
     </row>
-    <row r="491" spans="1:8">
+    <row r="491" spans="1:8" ht="12.75">
       <c r="A491" s="11"/>
       <c r="B491" s="10"/>
       <c r="C491" s="11"/>
@@ -5677,7 +5680,7 @@
       <c r="G491" s="12"/>
       <c r="H491" s="10"/>
     </row>
-    <row r="492" spans="1:8">
+    <row r="492" spans="1:8" ht="12.75">
       <c r="A492" s="11"/>
       <c r="B492" s="10"/>
       <c r="C492" s="11"/>
@@ -5687,7 +5690,7 @@
       <c r="G492" s="12"/>
       <c r="H492" s="10"/>
     </row>
-    <row r="493" spans="1:8">
+    <row r="493" spans="1:8" ht="12.75">
       <c r="A493" s="11"/>
       <c r="B493" s="10"/>
       <c r="C493" s="11"/>
@@ -5697,7 +5700,7 @@
       <c r="G493" s="12"/>
       <c r="H493" s="10"/>
     </row>
-    <row r="494" spans="1:8">
+    <row r="494" spans="1:8" ht="12.75">
       <c r="A494" s="11"/>
       <c r="B494" s="10"/>
       <c r="C494" s="11"/>
@@ -5707,7 +5710,7 @@
       <c r="G494" s="12"/>
       <c r="H494" s="10"/>
     </row>
-    <row r="495" spans="1:8">
+    <row r="495" spans="1:8" ht="12.75">
       <c r="A495" s="11"/>
       <c r="B495" s="10"/>
       <c r="C495" s="11"/>
@@ -5717,7 +5720,7 @@
       <c r="G495" s="12"/>
       <c r="H495" s="10"/>
     </row>
-    <row r="496" spans="1:8">
+    <row r="496" spans="1:8" ht="12.75">
       <c r="A496" s="11"/>
       <c r="B496" s="10"/>
       <c r="C496" s="11"/>
@@ -5727,7 +5730,7 @@
       <c r="G496" s="12"/>
       <c r="H496" s="10"/>
     </row>
-    <row r="497" spans="1:8">
+    <row r="497" spans="1:8" ht="12.75">
       <c r="A497" s="11"/>
       <c r="B497" s="10"/>
       <c r="C497" s="11"/>
@@ -5737,7 +5740,7 @@
       <c r="G497" s="12"/>
       <c r="H497" s="10"/>
     </row>
-    <row r="498" spans="1:8">
+    <row r="498" spans="1:8" ht="12.75">
       <c r="A498" s="11"/>
       <c r="B498" s="10"/>
       <c r="C498" s="11"/>
@@ -5747,7 +5750,7 @@
       <c r="G498" s="12"/>
       <c r="H498" s="10"/>
     </row>
-    <row r="499" spans="1:8">
+    <row r="499" spans="1:8" ht="12.75">
       <c r="A499" s="11"/>
       <c r="B499" s="10"/>
       <c r="C499" s="11"/>
@@ -5757,7 +5760,7 @@
       <c r="G499" s="12"/>
       <c r="H499" s="10"/>
     </row>
-    <row r="500" spans="1:8">
+    <row r="500" spans="1:8" ht="12.75">
       <c r="A500" s="11"/>
       <c r="B500" s="10"/>
       <c r="C500" s="11"/>

</xml_diff>